<commit_message>
update: added more generalised pathnames
</commit_message>
<xml_diff>
--- a/Excel/USA.xlsx
+++ b/Excel/USA.xlsx
@@ -11,6 +11,10 @@
     <sheet name="05-07-20 0921" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="07-07-20 0738" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="07-07-20 0741" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="07-07-20 0757" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="07-07-20 0802" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="07-07-20 0807" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="07-07-20 0813" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1934,7 +1938,1367 @@
           <t>https://www.sportscardforum.com/threads/2521884-WTTF-Team-USA-Cards</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>www.validdocumentsonline.com BUY REAL PASSPORTS / USA PASSPO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Source: Honda vt500 forumForum: Welcome</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>http://vt500-forum-uk.proboards.com/post/301/thread</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Welcome Guest. Please Login or Register.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RE:USA USA USA USA USA USA USA USA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Source: Where SRDines steal good drama from :)Forum: r/Drama</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Drama/comments/hl710m/usa_usa_usa_usa_usa_usa_usa_usa/fwxmmgr/</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>One more time for the commies in the backUSA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USAMembersOnline</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Paragraph</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>An American dream: Broadcasting AFL in the USA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>The Guardian</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.theguardian.com/sport/2020/jul/07/an-american-dream-broadcasting-afl-in-the-usa&amp;ct=ga&amp;cd=CAAYADIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNEZmUI53yb2cHlv3m53ZJFPA5n_2g</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>After the North American broadcast of the 1997 AFL grand final was delayed, a bunch of footy enthusiasts responded by buying the TV rightsJonathan HowcroftMon 6 Jul 2020 18.30 BST
+Last modified on Mon 6 Jul 2020E
+d Wyatt has the most interesting CV in Australian sport. As a TV host and radio commentator he has called or reported on it all, but fans of Australian basketball, baseball and football in particular will recognise his West Coast accent. Before that he won Emmys as a regular cast member of the sketch comedy show Almost Live! That was during his time in Seattle around the turn of the 1990s when the zeitgeist resided in the Pacific Northwest.In between those two lives Wyatt was part of a mob that bought the rights to broadcast the AFL in the USA, a story that includes the host of The Amazing Race, a star of Whose Line Is It Anyway, the brains behind BT Sport, and, most importantly of all, Wyatt’s wife, Michelle.With Australian sport bucking the global trend and providing some distraction from the pandemic there has been no shortage of attempts to recruit American viewers unfamiliar to Australian rules football. In light of this, the Wyatts recently revisited their own missionary project as part of The Greatest Season That Was podcast series.“It all came about because we wanted to watch the 1997 grand final between Adelaide and St Kilda on ESPN but the baseball that was on immediately beforehand went into extra innings, meaning the footy didn’t come on until midway through the opening quarter,” Wyatt explained to Guardian Australia. “No build-up, no anthems, and we were hosting a party at our place in Venice Beach, so we were furious.”In those days fury might have, at worst, led to a strongly worded letter to ESPN HQ, or the cancellation of a subscription, but the Wyatts were both employees of the recently launched Fox Sports World, giving them a platform to take more decisive action.Michelle Wyatt was a former producer of Channel Seven’s AFL coverage and the catalyst for the collective interest in the sport many miles from its heartland. Her Collingwood credentials go as far back as David Williamson’s seminal movie The Club where she appears in a crowd scene as a 12-year-old. She would later become the executive producer for Channel Ten’s popular series Before the Game.Michelle leveraged her contacts back in Australia to bring Fox Sports World into the conversation for securing AFL broadcast rights to avoid a repeat of the grand final debacle. Those negotiations were handled at the Los Angeles end by Simon Green who secured a three-year deal for one live game per week, one edited three-hour match, and one edited two-hour match. This was worth nothing to the AFL in year one, $40,000 in year two and $80,000 in year three. 15 years later Green was the driving force behind BT Sport shaking up coverage of the Premier League in the UK in a deal worth £246m per season.Fox Sports World only reached around 50,000 viewers by satellite, but the bigger carrot for the AFL was a route into America’s regional market under the umbrella of Fox Sports Net, where viewership jumped into the tens of millions. The campaign to grow subscribers mimicked the “I want my MTV” model of the 1980s with customers encouraged to call up their satellite provider at 1800 Fox World. Scripts to push this message via infomercials were written by Wyatt and voiced by Greg Proops and Phil Keoghan.After a near 20-year relationship with ESPN that had run out of steam, the AFL supported the new enterprise with priority access to players like Wayne Carey and James Hird, enabling the creation of a series of profiles and an A to Z of Australian rules primer. On trips back to Melbourne the Wyatts enjoyed an unfettered gameday experience, including the recording of links from the centre square of the MCG before the opening bounce. “Probably the most nervous I’ve ever been on television,” Wyatt recalls.The project peaked with the 1998 grand final. It was the first live broadcast accompanied by a dedicated pregame, hosted by Wyatt alongside the imported credentials of Gerard Healy. As part of the Fox Sports Net stable it was accessible in around 20 million homes.For all the ingenuity and talent involved the game didn’t take a quantum leap Stateside. Fox Sports World slashed its budget, while the obvious hook of Australian rules football to outsiders - the collisions and violence - was being legislated out of the game and downplayed for marketing purposes. But at least there was no longer baseball stopping play. “I think we delivered,” said Wyatt.The Wyatts relocated to Melbourne in 1999, mission somewhat accomplished. The AFL in the US has since gone full circle, first leaving Fox Sports World, spending a long time on the Setanta network, before eventually returning to Fox; still a niche offering, still with unrealised potential, still often viewed with mock-horror by disbelieving Americans wondering who forgot to bring the shoulder pads.“We were maybe ahead of our time,” Michelle Wyatt considers. With US networks still short of live sport to broadcast (turning recently to Adelaide v Fremantle as primetime fodder), and sports radio hosts clamouring for anything to get excited about, that groundwork may, belatedly, be coming to fruition.Hear more in The Greatest Season That Was Presents... we have a small favour to ask. Millions are flocking to the Guardian for quality news every day. We believe everyone deserves access to factual information, and analysis that has authority and integrity. That’s why, unlike many others, we made a choice: to keep Guardian reporting open for all, regardless of where they live or what they can afford to pay.As an open, independent news organisation we investigate, interrogate and expose the actions of those in power, without fear. With no shareholders or billionaire owner, our journalism is free from political and commercial bias – this makes us different. We can give a voice to the oppressed and neglected, and stand in solidarity with those who are calling for a fairer future. With your help we can make a difference.We’re determined to provide journalism that helps each of us better understand the world, and take actions that challenge, unite, and inspire change – in times of crisis and beyond. Our work would not be possible without our readers, who now support our work from 180 countries around the world.But news organisations are facing an existential threat. With advertising revenues plummeting, the Guardian risks losing a major source of its funding. More than ever before, we’re reliant on financial support from readers to fill the gap. Your support keeps us independent, open, and means we can maintain our high quality reporting – investigating, disentangling and interrogating.Every reader contribution, however big or small, is so valuable for our future. Support the Guardian from as little as $1 – and it only takes a minute. Thank you.Sign in or create your Guardian account to join the discussion.14 comments in and half of them are from bitter Australian soccer fans....more comments than most articles on Australian soccer can musterImagine if their passionate hatred and jealousy at Australian football could be channelled positively into Australian soccer?The only sport you get a point for missingWe and our partners use your information – collected through cookies and similar technologies – to improve your experience on our site, analyse how you use it and show you personalised advertising.You can find out more in our privacy policy and cookie policy, and manage your consent at any time by going to ‘Privacy settings’ at the bottom of any page.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Coronavirus USA live news summary for Sunday July 5th</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>AS English</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://en.as.com/en/2020/07/05/latest_news/1593903056_351097.html&amp;ct=ga&amp;cd=CAAYATIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNGZrBLz0VsZSBOt__pL_w-p1CpxMQ</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Latest NewsAS ENGLISHAccording to the latest figures published by John Hopkins University, 11,565,414 cases have been detected worldwide, with 536,650 deaths and 6,231,052 people recovered.In the USA, there have been 2,922,000 confirmed cases and 130,208 deaths, with 924,148 people recovered from the virus.It feels like, with Florida seeing a massive surge in cases, that this is not the best way to go about curbing the spread.Ventures backed by big-name entertainers Kanye West and Francis Ford Coppola were among those approved for loans under a U.S. government program to help businesses survive the coronavirus pandemic, according to a list released on Monday.Billionaire rapper West's clothing brand Yeezy received clearance for a loan of between $2 million and $5 million under the Paycheck Protection Program, the U.S. Small Business Administration said.The company said the loan would save 160 jobs, according to the SBA.The PPP was established to aid workers at companies and nonprofits with fewer than 500 employees hurt by closures and other measures meant to slow the spread of the novel coronavirus. The list released Monday gave the most-detailed accounting to date of who applied for and was approved to receive funds.US NEWSTrump Rallies for the 2020 presidential elections in the United States: schedule, dates and places42 states now seeing daily rises.Coronavirus has touched every aspect of American life. This US Covid-19 recovery hub will give you the data to measure where recovery is happening as it happens.With the news that there was a suspected case in China, questions were raised about what it could mean as we fight with the Covid-19 pandemic.CORONAVIRUSWhat is the bubonic plague, its symptoms and how it spreads?The Post looks at how Dr Fauci and others manage their lives amid the dangers of the current pandemic.In the span of a week and a half, the number of coronavirus cases in the United States has doubled, yet officials are saying this is still the first wave of the pandemic.Atlanta Mayor Keisha Lance Bottoms said on Monday that she has tested positive for Covid-19, but has not shown symptoms of the virus.She gave no information about her diagnosis, whether she is under quarantine and when she was tested. 'Covid-19 has literally hit home,' the first-term mayor of Georgia's state capital city said on Twitter.In New York, site of the country's largest outbreak, the state's curve rose sharply before reaching over 170,000 total cases in April. Since then, new cases have fallen from about 10,000 per day in mid-April to fewer than 700 per day in late June.Here are some of the stories that were making the headlines over the last 24 hours:- San Diego County was officially added to California's "monitoring list"- Sen. Grassley says he will skip Republican convention due to coronavirus concerns- MLB confirms testing delays, doesn't expect recurrence- Tiafoe out of World TeamTennis after positive test- Coronavirus hospitalizations grow in more than 20 states as Texas admissions soar to new record- Trump plans New Hampshire rally as he works to re-energize campaignAccording to the latest figures published by John Hopkins University, 11,565,414 cases have been detected worldwide, with 536,650 deaths and 6,231,052 people recovered.In the USA, there have been 2,922,000 confirmed cases and 130,208 deaths, with 924,148 people recovered from the virus.More than 11.5 million people globally have contracted the disease according to official figures, and well over half a million have lost their lives to the virus since it started to spread at the beginning of the year.In the US, the first wave was believed to be over but that is obviously not the case.Texas, Florida, Arizona and California have seen a resurgence in new cases and record numbers of hospitalisations reaffirming fears that a second wave, or a continuation of the first, is a very real possibility..0
+ComentariosEdiciones internacionalesAppsSíguenos© DIARIO AS, S.L. - Valentín Beato, 44 - 28037 Madrid [España] - Tel. 91 375 25 00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Chris Moffett joins USA Groups</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Yahoo Finance</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/news/chris-moffett-joins-usa-groups-130000169.html&amp;ct=ga&amp;cd=CAAYAjIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNF8y66blO66kc8vXVUw1QkFjkk34w</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>SARASOTA, Fla., July 6, 2020 /PRNewswire/ -- Today, USA Groups, Inc. announced that Chris Moffett is joining the communications infrastructure firm as its new Chief Executive Officer. Moffett brings with him an extensive background in executive management, leadership, mergers and acquisitions, and strategic planning.  Moffett's knowledge of the communications industry will enable USA Groups to modify its unique product and service offerings."I could not be happier about bringing Chris into the USA Groups family.  For over 25 years the management team has positioned us as a leader in telecommunications construction and engineering by focusing on our customers' needs and then executing in a disciplined manner to consistently meet those needs," said James Goff, Executive Chairman (and now former CEO) of USA GROUPS.  "We are confident that Chris can accelerate our growth both organically and through strategic acquisitions.""I feel blessed to have been asked to lead USA Groups in its next phase of growth," stated
+Moffett.  "USA delivers a unique blend of products and services that are essential for the communications industry to deliver next generation networks.  USA Groups has a seasoned team of industry experts and I am excited to work with them to industrialize our offerings so that we can play an even larger role in helping our customers be successful."Moffett has 20 years of experience at Crown Castle International Corp. His prior roles included Director of International Acquisitions, Director of Commercial Strategy, Director of Finance and culminated with him being the President of Crown Castle's South Area for 14 years where he had P&amp;L responsibility for $1.3B in revenue, oversaw 11,000 macro sites, 20,000 small cell nodes and managed roughly 450 employees. Moffett holds a BSM in Finance and Marketing from Tulane University as well master's degrees in International Finance from The London School of Economics and Political Science as well as ASU's Thunderbird School of Global Management.About USA GROUPS
+USA GROUPS is a leading provider of construction, engineering and fabricated steel products to the telecommunications and infrastructure industries. These services, which are provided throughout the United States, include construction management, tower construction and modifications, engineering, structural steel fabrication, surveying, installation, and maintenance services to telecommunications providers, developers and government clients.  For more information on USA Groups, please visit www.usa-groups.com.Contact:
+Katie Kinnetz
+(800) 541-2170View original content to download multimedia:http://www.prnewswire.com/news-releases/chris-moffett-joins-usa-groups-301088331.htmlSOURCE USA Groups, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>RE:ブルーススプリングスティーンの大ヒット曲 『Born in the USA』の歌詞の中で 『ベトナムに黄色い猿を殺しに行く』ってフレーズが あるんですけど、スプリングスティーンさんて 人種差別主...</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Source: カテゴリ一覧 - Yahoo!知恵袋Forum: 洋楽</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://detail.chiebukuro.yahoo.co.jp/qa/question_detail/q14227811489</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>三陸の「牛乳瓶生ウニ」や殻付きウニなど、逸品をお取り寄せ検索IDでもっと便利に新規取得ログインお買い物がお得になるクーポンがたくさん条件指定質問・相談回答受付終了まであと4日　回答を投稿すると知恵コイン15枚が追加されますシェアツイートはてブ知恵コレID非公開さん2020/7/312:35:55ブルーススプリングスティーンの大ヒット曲
+『Born in the USA』の歌詞の中で
+『ベトナムに黄色い猿を殺しに行く』ってフレーズが
+あるんですけど、スプリングスティーンさんて人種差別主義者なんですか？違反報告回答投稿シェアツイートはてブ知恵コレ1〜5件/5件中猿メガネさん編集あり2020/7/517:01:15仮に黄色い猿と歌ってたとしても
+前後の文脈をしっかり聴けば
+人種差別主義者なんかでは
+ないことが理解できるはず。
+ある単語やフレーズだけを抜き出して
+過剰に反応する
+リテラシー能力のない人が
+最近は多いみたいやけど。違反報告kus********さん2020/7/319:45:27妄想が過ぎます違反報告不適切な内容が含まれている可能性があるため、非表示になっています。投稿内容に関する注意つぃんどっぐさん2020/7/314:41:04Got in a little hometown jam so they put rifle in my hand.
+Sent me off to a foriegan land to go and kill the yellow man.
+Born in the U.S.A.
+I was born in the U.S.A.
+.....
+どこにもyellow monkyとは書いてないが?違反報告質問者ID非公開さん2020/7/315:16:53Got in a little hometown jam
+So they put a rifle in my hand
+Sent me off to a foreign land
+To go and kill the yellow mon
+https://blog.goo.ne.jp/kantenbou/e/3bb6da51509f89f43922a62d2371fc7f
+書いてるじゃないか？違反報告その他の返信（2件）を表示ave********さん2020/7/312:48:03「黄色い猿」なんて歌っていません、「黄色い人間」の間違いです。
+人種をイエローというのは、そんなに差別的じゃないでしょう。違反報告一覧を見るみんなで作る知恵袋　悩みや疑問、なんでも気軽にきいちゃおう！Q&amp;Aをキーワードで検索：ランキングをもっと見る一覧を見るエンターテインメントと趣味∟音楽JASRAC許諾番号：9008249113Y38200Copyright (C) 2020 Yahoo Japan Corporation. All Rights Reserved.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RE:Since the USA ranks like 12th ..</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Source: URG Conversations - Ur Energy Inc Common Shares (Ca - Yahoo FinanceForum: UR-Energy Inc. (URG)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://finance.yahoo.com/quote/URG/community</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.5400 +0.01 (1.22%)
+After hours: 6:27PM EDT</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Re: Anytown, USA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Source: The Motley Fool Discussion BoardsForum: Political Asylum</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://boards.fool.com/Message.aspx?mid=34552208&amp;sort=whole</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Folders | Best Of | Favorites &amp; Replies | Settings | Start a New Board | My Fool | Help |© 1995 - 2020 The Motley Fool. All rights reserved.
+Market data powered by FactSet and Web Financial Group.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>www.validdocumentsonline.com BUY REAL PASSPORTS / USA PASSPO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Source: AboutAlcoholismForum: Stories &amp; Journals</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>http://aboutalcoholism.proboards.com/post/5184/thread</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Welcome Guest. Please Login or Register.Welcome Guest. Please Login or Register.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>WTTF: Team USA Cards</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Source: Sports Card Trading and Sports Card ForumForum: Most Recent SCF Posts</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://www.sportscardforum.com/threads/2521884-WTTF-Team-USA-Cards</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>www.validdocumentsonline.com BUY REAL PASSPORTS / USA PASSPO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Source: Honda vt500 forumForum: Welcome</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>http://vt500-forum-uk.proboards.com/post/301/thread</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Welcome Guest. Please Login or Register.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RE:USA USA USA USA USA USA USA USA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Source: Where SRDines steal good drama from :)Forum: r/Drama</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Drama/comments/hl710m/usa_usa_usa_usa_usa_usa_usa_usa/fwxmmgr/</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>One more time for the commies in the backUSA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USAOne good thing to come out of this banwave stuff is that so many of these banned communities are making their own dedicated sites. Incels and T_D have had their sites for ages now, now you have radfems, femcels, and even cumboys going to their own sites/forums. Except of course chapos who have to once again prove to be a massive disappointment by going to that leftoid gab (raddle?) instead of making their own brand new site like everyone else. I imagine most of these sites are going to die out, but it would be nice if admins of massive sites kept going "NO FUN ALLOWED", leading to more and more communities bailing out and starting a forum renaissance.Oh yeah also thanks for reading my blog boys girls and everyone else.Actress and model Molly Conlin, 19, who starred in British soap opera EastEnders, claimed on Twitter that she was attacked in her home by a gang of "tall black men" who "barged in" and pinned her down on the ground as they robbed her.This image shows her original Twitter posts. Here's a Sun article reporting on her account of the incident.People soon noticed that Molly's social media was filled with seeming to support the BlackLivesMatter movement, demanding racial justice and attacking police as racist killers.MembersOnline</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Paragraph</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>An American dream: Broadcasting AFL in the USA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>The Guardian</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.theguardian.com/sport/2020/jul/07/an-american-dream-broadcasting-afl-in-the-usa&amp;ct=ga&amp;cd=CAAYADIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNEZmUI53yb2cHlv3m53ZJFPA5n_2g</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>After the North American broadcast of the 1997 AFL grand final was delayed, a bunch of footy enthusiasts responded by buying the TV rightsE
+d Wyatt has the most interesting CV in Australian sport. As a TV host and radio commentator he has called or reported on it all, but fans of Australian basketball, baseball and football in particular will recognise his West Coast accent. Before that he won Emmys as a regular cast member of the sketch comedy show Almost Live! That was during his time in Seattle around the turn of the 1990s when the zeitgeist resided in the Pacific Northwest.In between those two lives Wyatt was part of a mob that bought the rights to broadcast the AFL in the USA, a story that includes the host of The Amazing Race, a star of Whose Line Is It Anyway, the brains behind BT Sport, and, most importantly of all, Wyatt’s wife, Michelle.With Australian sport bucking the global trend and providing some distraction from the pandemic there has been no shortage of attempts to recruit American viewers unfamiliar to Australian rules football. In light of this, the Wyatts recently revisited their own missionary project as part of The Greatest Season That Was podcast series.“It all came about because we wanted to watch the 1997 grand final between Adelaide and St Kilda on ESPN but the baseball that was on immediately beforehand went into extra innings, meaning the footy didn’t come on until midway through the opening quarter,” Wyatt explained to Guardian Australia. “No build-up, no anthems, and we were hosting a party at our place in Venice Beach, so we were furious.”In those days fury might have, at worst, led to a strongly worded letter to ESPN HQ, or the cancellation of a subscription, but the Wyatts were both employees of the recently launched Fox Sports World, giving them a platform to take more decisive action.Michelle Wyatt was a former producer of Channel Seven’s AFL coverage and the catalyst for the collective interest in the sport many miles from its heartland. Her Collingwood credentials go as far back as David Williamson’s seminal movie The Club where she appears in a crowd scene as a 12-year-old. She would later become the executive producer for Channel Ten’s popular series Before the Game.Michelle leveraged her contacts back in Australia to bring Fox Sports World into the conversation for securing AFL broadcast rights to avoid a repeat of the grand final debacle. Those negotiations were handled at the Los Angeles end by Simon Green who secured a three-year deal for one live game per week, one edited three-hour match, and one edited two-hour match. This was worth nothing to the AFL in year one, $40,000 in year two and $80,000 in year three. 15 years later Green was the driving force behind BT Sport shaking up coverage of the Premier League in the UK in a deal worth £246m per season.Fox Sports World only reached around 50,000 viewers by satellite, but the bigger carrot for the AFL was a route into America’s regional market under the umbrella of Fox Sports Net, where viewership jumped into the tens of millions. The campaign to grow subscribers mimicked the “I want my MTV” model of the 1980s with customers encouraged to call up their satellite provider at 1800 Fox World. Scripts to push this message via infomercials were written by Wyatt and voiced by Greg Proops and Phil Keoghan.After a near 20-year relationship with ESPN that had run out of steam, the AFL supported the new enterprise with priority access to players like Wayne Carey and James Hird, enabling the creation of a series of profiles and an A to Z of Australian rules primer. On trips back to Melbourne the Wyatts enjoyed an unfettered gameday experience, including the recording of links from the centre square of the MCG before the opening bounce. “Probably the most nervous I’ve ever been on television,” Wyatt recalls.The project peaked with the 1998 grand final. It was the first live broadcast accompanied by a dedicated pregame, hosted by Wyatt alongside the imported credentials of Gerard Healy. As part of the Fox Sports Net stable it was accessible in around 20 million homes.For all the ingenuity and talent involved the game didn’t take a quantum leap Stateside. Fox Sports World slashed its budget, while the obvious hook of Australian rules football to outsiders - the collisions and violence - was being legislated out of the game and downplayed for marketing purposes. But at least there was no longer baseball stopping play. “I think we delivered,” said Wyatt.The Wyatts relocated to Melbourne in 1999, mission somewhat accomplished. The AFL in the US has since gone full circle, first leaving Fox Sports World, spending a long time on the Setanta network, before eventually returning to Fox; still a niche offering, still with unrealised potential, still often viewed with mock-horror by disbelieving Americans wondering who forgot to bring the shoulder pads.“We were maybe ahead of our time,” Michelle Wyatt considers. With US networks still short of live sport to broadcast (turning recently to Adelaide v Fremantle as primetime fodder), and sports radio hosts clamouring for anything to get excited about, that groundwork may, belatedly, be coming to fruition.Hear more in The Greatest Season That Was PresentsWe and our partners use your information – collected through cookies and similar technologies – to improve your experience on our site, analyse how you use it and show you personalised advertising.You can find out more in our privacy policy and cookie policy, and manage your consent at any time by going to ‘Privacy settings’ at the bottom of any page.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chris Moffett joins USA Groups</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Yahoo Finance</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/news/chris-moffett-joins-usa-groups-130000169.html&amp;ct=ga&amp;cd=CAAYATIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNF8y66blO66kc8vXVUw1QkFjkk34w</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SARASOTA, Fla., July 6, 2020 /PRNewswire/ -- Today, USA Groups, Inc. announced that Chris Moffett is joining the communications infrastructure firm as its new Chief Executive Officer. Moffett brings with him an extensive background in executive management, leadership, mergers and acquisitions, and strategic planning.  Moffett's knowledge of the communications industry will enable USA Groups to modify its unique product and service offerings."I could not be happier about bringing Chris into the USA Groups family.  For over 25 years the management team has positioned us as a leader in telecommunications construction and engineering by focusing on our customers' needs and then executing in a disciplined manner to consistently meet those needs," said James Goff, Executive Chairman (and now former CEO) of USA GROUPS.  "We are confident that Chris can accelerate our growth both organically and through strategic acquisitions.""I feel blessed to have been asked to lead USA Groups in its next phase of growth," stated
+Moffett.  "USA delivers a unique blend of products and services that are essential for the communications industry to deliver next generation networks.  USA Groups has a seasoned team of industry experts and I am excited to work with them to industrialize our offerings so that we can play an even larger role in helping our customers be successful."Moffett has 20 years of experience at Crown Castle International Corp. His prior roles included Director of International Acquisitions, Director of Commercial Strategy, Director of Finance and culminated with him being the President of Crown Castle's South Area for 14 years where he had P&amp;L responsibility for $1.3B in revenue, oversaw 11,000 macro sites, 20,000 small cell nodes and managed roughly 450 employees. Moffett holds a BSM in Finance and Marketing from Tulane University as well master's degrees in International Finance from The London School of Economics and Political Science as well as ASU's Thunderbird School of Global Management.About USA GROUPS
+USA GROUPS is a leading provider of construction, engineering and fabricated steel products to the telecommunications and infrastructure industries. These services, which are provided throughout the United States, include construction management, tower construction and modifications, engineering, structural steel fabrication, surveying, installation, and maintenance services to telecommunications providers, developers and government clients.  For more information on USA Groups, please visit www.usa-groups.com.Contact:
+Katie Kinnetz
+(800) 541-2170View original content to download multimedia:http://www.prnewswire.com/news-releases/chris-moffett-joins-usa-groups-301088331.htmlSOURCE USA Groups, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Coronavirus USA live updates: cases, deaths, news and stimulus checks, today, July 6th</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AS English</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://en.as.com/en/2020/07/06/latest_news/1593989092_414237.html&amp;ct=ga&amp;cd=CAAYAjIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNECgIKply8r6NwGfj08Yc25baXwBg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Latest NewsAS ENGLISHAccording to the latest figures published by John Hopkins University, 11,565,414 cases have been detected worldwide, with 536,650 deaths and 6,231,052 people recovered.In the USA, there have been 2,922,000 confirmed cases and 130,208 deaths, with 924,148 people recovered from the virus.It feels like, with Florida seeing a massive surge in cases, that this is not the best way to go about curbing the spread.Ventures backed by big-name entertainers Kanye West and Francis Ford Coppola were among those approved for loans under a U.S. government program to help businesses survive the coronavirus pandemic, according to a list released on Monday.Billionaire rapper West's clothing brand Yeezy received clearance for a loan of between $2 million and $5 million under the Paycheck Protection Program, the U.S. Small Business Administration said.The company said the loan would save 160 jobs, according to the SBA.The PPP was established to aid workers at companies and nonprofits with fewer than 500 employees hurt by closures and other measures meant to slow the spread of the novel coronavirus. The list released Monday gave the most-detailed accounting to date of who applied for and was approved to receive funds.US NEWSTrump Rallies for the 2020 presidential elections in the United States: schedule, dates and places42 states now seeing daily rises.Coronavirus has touched every aspect of American life. This US Covid-19 recovery hub will give you the data to measure where recovery is happening as it happens.With the news that there was a suspected case in China, questions were raised about what it could mean as we fight with the Covid-19 pandemic.CORONAVIRUSWhat is the bubonic plague, its symptoms and how it spreads?The Post looks at how Dr Fauci and others manage their lives amid the dangers of the current pandemic.In the span of a week and a half, the number of coronavirus cases in the United States has doubled, yet officials are saying this is still the first wave of the pandemic.Atlanta Mayor Keisha Lance Bottoms said on Monday that she has tested positive for Covid-19, but has not shown symptoms of the virus.She gave no information about her diagnosis, whether she is under quarantine and when she was tested. 'Covid-19 has literally hit home,' the first-term mayor of Georgia's state capital city said on Twitter.In New York, site of the country's largest outbreak, the state's curve rose sharply before reaching over 170,000 total cases in April. Since then, new cases have fallen from about 10,000 per day in mid-April to fewer than 700 per day in late June.Here are some of the stories that were making the headlines over the last 24 hours:- San Diego County was officially added to California's "monitoring list"- Sen. Grassley says he will skip Republican convention due to coronavirus concerns- MLB confirms testing delays, doesn't expect recurrence- Tiafoe out of World TeamTennis after positive test- Coronavirus hospitalizations grow in more than 20 states as Texas admissions soar to new record- Trump plans New Hampshire rally as he works to re-energize campaignAccording to the latest figures published by John Hopkins University, 11,565,414 cases have been detected worldwide, with 536,650 deaths and 6,231,052 people recovered.In the USA, there have been 2,922,000 confirmed cases and 130,208 deaths, with 924,148 people recovered from the virus.More than 11.5 million people globally have contracted the disease according to official figures, and well over half a million have lost their lives to the virus since it started to spread at the beginning of the year.In the US, the first wave was believed to be over but that is obviously not the case.Texas, Florida, Arizona and California have seen a resurgence in new cases and record numbers of hospitalisations reaffirming fears that a second wave, or a continuation of the first, is a very real possibility..0
+ComentariosEdiciones internacionalesAppsSíguenos© DIARIO AS, S.L. - Valentín Beato, 44 - 28037 Madrid [España] - Tel. 91 375 25 00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>'Grim resolve': Biden is up big and the Senate is in sight, but Democrats still haunted by fear of ...</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>USA TODAY</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.usatoday.com/story/news/politics/2020/07/05/joe-biden-up-big-and-senate-grasps-dems-haunted-fear-letdown/3284392001/&amp;ct=ga&amp;cd=CAAYBDIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNFVqXUXUEbGe2k2YcqJQm1uoXyndA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>WASHINGTON – Democrats have heard this story before.Their standard-bearer builds a sizable lead in the race for president against Donald Trump. Everything seems pointed in their direction. Pundits talk about a Democratic victory like it’s inevitable. Then it doesn’t happen.Still licking their wounds four years after Hillary Clinton’s stinging loss, Democrats are grappling with heightened expectations that didn’t seem possible at the start of the year. Presumptive Democratic nominee Joe Biden cruised to a double-digit lead nationally weeks ago and has stayed there as President Trump takes a pounding over his handling of the coronavirus crisis, high unemployment and the fallout from nationwide protests over police brutality.Not only does Biden lead polls in every battleground state – a wider command than Clinton ever had – the former vice president is either ahead or competitive in states that the GOP must carry, including Texas, Georgia, Iowa, Ohio and Missouri. Democrats also have a path to take control of the Senate.More:Trump trails Biden in Michigan, Wisconsin, Pennsylvania, Florida, North Carolina and Arizona, poll findsOn one hand, Democrats are gushing about their prospects: a chance for a sweeping victory, not just eking out a win, to deliver a clear repudiation of the Trump era and unseat Mitch McConnell as Senate majority leader.But they’re not able to shake off their painful memories of 2016, when many Democrats falsely assumed that the Republican Party’s nomination of a reality TV show host with no elected office experience would ensure a Clinton victory in November."That memory can't be erased," said Luis Heredia, executive director of the Arizona Education Association, the state's teachers union, and a Democratic National Committee member. He recalled watching swing states Pennsylvania and Michigan quickly collapse for Democrats on election night. “That memory is still very fresh, especially for me.”"You remind people that a poll is just a poll," Heredia said. "It's a moment in time on Tuesday morning when somebody answered a call. Let's not get carried away. We should be winning by 20 points, given the circumstances. Winning by 6 points is still too close for us to say that we're ahead of the game."In interviews with DNC members from six battleground states, including party leaders, each came back to an old campaign cliche: “Take nothing for granted.”Democratic anxiety is assuaged a bit by the different circumstances this time around: Trump is an incumbent, unable to run as a businessman outsider fighting to “drain the swamp.” Multiple crises – including a pandemic that’s resulted in more than 129,000 American deaths – are part of his record. He just wrapped up arguably the most difficult month in his presidency, capped by a controversy over reports that Russia offered bounties to the Taliban to kill U.S. soldiers.More:Trump denies knowing about intelligence report that Russia put bounty on US troops in AfghanistanPerhaps most significantly, Biden lacks the low favorability and trustworthiness marks that doomed Clinton, whose polarization gave Trump an opening many Democrats did not see.There is a major warning sign for Democrats: Despite Biden’s sizable lead, his supporters are significantly less enthusiastic about him than Trump’s loyalists are of the president, polling shows.“Democrats across Wisconsin have two reactions to this moment,” said Ben Wikler, chairman of the Wisconsin Democratic Party. “The first is that Trump is an unmitigated disaster, and polls demonstrate that everyone knows he’s bad. The second reaction is that we have learned our lesson from 2016.”He said Democrats “can’t take their foot off the gas even for a second” by buying too much into the polls, noting that Clinton led Trump by as many as 15 percentage points in Wisconsin after the Democratic National Convention in August 2016. Trump ended up winning Wisconsin by less than 1 percentage point.“I would encapsulate it as ‘grim resolve,’ ” Wikler said of the mood among Democrats. It’s “mystifying that Trump even has the scraps of support he has,” given his troubles. He said Democrats fear Trump is “willing to cheat his way back into power” by limiting voter access and refusing to accept results.More:Biden and Trump each warn that other side may 'steal' the election as fight over mail voting ragesThere are four months left before the election, enough time for the race to upend again.“The thing that keeps me up at night is the unknown unknowns,” Wikler said.Trump’s wins in Wisconsin, Michigan and Pennsylvania, three pivotal states that historically vote Democratic, proved fatal for Clinton in 2016. Winning back the Rust Belt is key for Biden, who holds a polling lead of 6 points or more in each state, according to the Real Clear Politics average of polls.Democratic leaders in these states said they began rebuilding campaign infrastructure quickly after their 2016 defeats in preparation for 2020.“I don’t think anybody is comfortable with these numbers,” said Lavora Barnes, chairwoman of the Michigan Democratic Party. “There were people in 2016 who, very early on, because of who Donald Trump was, thought, ‘How could this nation possibly choose Donald Trump?’ Now that that’s happened, we recognize that we should never count anybody out.”Barnes said the Clinton campaign started focusing on Michigan “late,” after the party conventions in the late summer, but the Biden campaign is already working closely with the state party’s operations.“We all recognize the importance of this moment and the opportunities here, but they are only opportunities for us if we take advantage of them by doing the work,” she said.Rick Bloomingdale, president of the Pennsylvania AFL-CIO and a DNC committee member, said Biden’s strong numbers show that workers are worried about the economy and the pandemic, and “they’re seeing no leadership from Washington, D.C.”“But that doesn't mean they're going to hold. Trump has shown an incredible ability to be down and then back up. A lot can happen in those (final 120) days. In 2016, people thought, 'Oh man, if they nominate Trump, this thing's a waltz.' It wasn't, of course. We shouldn't assume it's going to be this time."He said, "We'd all love for the election to be over today. But we also know that's not the case.”Asked whether he feels good about Biden carrying Pennsylvania, Bloomingdale said, “I was confident that Hillary was going to win Pennsylvania. If we do the work, we’ll win. If we don’t do the work, we won’t win.”Wikler said Democrats in Wisconsin “erased” the advantage an incumbent typically has by laying groundwork since 2017.Like Michigan and Pennsylvania, Trump carried Wisconsin with strong support from white, working-class voters, winning rural counties across the state with more than 60% of the vote. Since then, Wikler noted, Sen. Tammy Baldwin, D-Wis., won her reelection in 2018 by double digits. Wikler said he believes Biden can make more inroads in rural areas where farms have been hurt by Trump’s trade policies.“We know that Trump is targeting Wisconsin as an absolute-must state for reelection,” Wikler said. “For us, that means we have to fight for every vote, and we’re investing accordingly.”Biden leads Trump nationally, 53%-41%, according to a USA TODAY/Suffolk University poll released last week, and holds a 9.4% lead in the Real Clear Politics average of polls.At this juncture in 2016, Clinton’s advantage over Trump was smaller, 46%-40% in the USATODAY/Suffolk poll, and Trump started to close the gap. In the Real Clear Politics average of polls on July 1, 2016, Clinton led by 4.8 points, a tightening from her double-digit advantage in the spring.Exclusive USA TODAY poll: Biden widens his lead, but Trump keeps the edge on enthusiasmAlthough some slammed the accuracy of polling after Trump won in an upset, Clinton's final lead in the popular vote, 48.2% to 46.1%, closely matched final polls. Trump's edge in the Electoral College came from close wins in swing states.Troubling for Trump this go-around: Only 20% of voters surveyed in the USA TODAY poll say the USA is headed in the right direction. The majority (67%) say the country is headed in the wrong direction. Biden also lacks the same negatives as Clinton, including questions over character.Fifty percent of voters surveyed say they find Biden honest and trustworthy, compared with 30% for Trump. Six weeks before the 2016 election, Trump led the trustworthy question. A Washington Post/ABC poll found 33% of voters found Clinton honest and trustworthy, and Trump was trusted by 42%.David Paleologos, director of Suffolk University’s Political Research Center, said the 2016 electorate was swung by “the haters” – voters who disliked both Trump and Clinton. He said the “intensity against Hillary Clinton ended up being higher than Trump, especially in the swing states.” Trump benefited by a race that turned highly negative because Clinton was more polarizing. “This year, you don’t have that,” Paleologos said. “He’s likable. He’s likable Joe.”Paleologos on the poll: First, we couldn't talk politics at Thanksgiving. Now, the 4th?For Trump, Paleologos said, “that’s really the challenge ahead. He doesn’t have an opponent who people hate or have a visceral reaction to.”Biden’s biggest vulnerability could be the enthusiasm gap. Most of his supporters back him because he’s “not Trump,” according to Paleologos. Half of Trump's backers say they are "very excited" about their candidate; 27% of Biden backers say that. “The people for Trump, they love him. The people for Biden, they shrug their shoulders,” Paleologos said.Biden leads overwhelmingly among voters not enthusiastic about either candidate. “That’s right now taking its toll on the Trump campaign,” Paleologos said.Biden downplayed his lead during his first news conference since April after a speech last week in Wilmington, Delaware. He was asked about his unorthodox campaign, which has operated largely from his home in Delaware during the pandemic. Biden said “the irony” is he’s probably been able to reach more voters through virtual campaigning.“So far, it remains to be seen, I don’t want to jinx myself, I know the polling data is very good. But I think it’s really early. It’s much too early to make any judgment,” Biden said.Biden in the basement: Can campaigning from home work as Trump starts to travel?Trump and Republicans have struggled to find an attack against Biden that’s stuck.During a conference call with reporters, Trump communication director Tim Murtaugh threw the gauntlet at Biden.He slammed Biden for not denouncing the tear-downs of monuments by protesters, called him a “disaster” on the economy, talked extensively about Rep. Alexandria Ocasio-Cortez, D-N.Y., questioned Biden’s ties to China and argued the Obama-Biden administration’s handling of the H1N1 pandemic left Trump with a shortage of N95 masks. He accused Biden of using COVID-19 as a “political weapon in a cynical attempt” to undermine public confidence.“Joe Biden is hoping to ride out the rest of these four months without taking any of these questions,” Murtaugh said. “He’s not undergoing thorough vetting before the American people, and he’s not facing scrutiny because his handlers know he is not up to it.”Comparing the 2020 and 2016 elections, Robby Mook, Clinton's 2016 campaign manager, said last week, “I almost look at it as: Is there very much that’s the same?” He appeared on the podcast of David Plouffe, Barack Obama’s former campaign manager. “First and foremost, I’d say COVID has changed everything.”Mook, president of the House Majority PAC, said Trump is taken "more seriously" and "being held to account in a way that he wasn’t in ’16.” Whereas Trump’s "petty" remarks were treated as a “novelty” in 2016, they’re now seen “in a context of a true lack of leadership,” he said. Political experience tends to be a liability in campaigns, Mook said, but it’s viewed as a strength for Biden during the pandemic. “I think Hillary kind of got the opposite end of that." He predicted the race would tighten up as voters, as they historically do, "go home to their parties," but not if Trump can't "get his act together."“Biden wants this to be a referendum on Trump, and he’s winning that right now. Trump needs to reengineer that to be a choice – and he can’t even offer what that choice is," Mook said. "So how in the world are they supposed to get this on firmer ground for their strategy?”None of the Trump taglines on Biden has gained traction like “Crooked Hillary” and chants of “Lock her up” four years ago.Democrats, despite their cautious optimism, are bullish about the issues being in their favor: a pandemic they contend exposed failed presidential leadership and Trump's “law and order” response to protests over systemic racism and police brutality as polling shows more Americans are favorable to the Black Lives Matter movement. "We understand what the temperature and the pulse of the country looks like right now,” said Shelia Huggins, an attorney from Durham, North Carolina, and DNC committee member.More:Joe Biden campaign seizes on opportunity to contrast Trump's 'law and order' messageShe said her Democratic friends aren’t talking about a 2016 repeat as much as they once were."We’re too busy listening to a president who is talking nonsense pretty much every day,” she said. “You're easily reminded that 2016 is not what needs to be on the forefront of what we're thinking about. We need to be thinking about 2020."In Arizona, Heredia said he believes Democrats have momentum to carry the state for Biden, win the U.S. Senate race between Democrat Mark Kelly and Sen. Martha McSally and flip both chambers of the state Legislature, where Republicans have slim majorities. The last Democrat to carry Arizona for president was Bill Clinton in 1996. “There's a perfect storm building up in Arizona, I would call it a perfect ‘haboob’ in our state,” he said, referring to the dust storms that pop up in the SouthwestMore:Trump calls proposed Black Lives Matter mural outside Trump Tower 'a symbol of hate'Ken Evans, a DNC committee member from Florida, who runs a camp for children in Fort Lauderdale, said he knows many "nonpartisan people" in Broward County who voted for Trump because they couldn’t back Clinton, but they plan to vote for Biden in November. He said the president’s handling of the coronavirus was the last straw.“That’s making the difference. That’s what’s going to bring out the vote,” Evans said, defending voter enthusiasm for Biden. “They’re excited to bring normalcy back to the White House” after all the "tiresome" Trump drama, he said. “People are tired.”When it comes to Biden being ahead in polls, though, Evans returned to four years ago.“So was Hillary, right?” he said.Reach Joey Garrison on Twitter @joeygarrison.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RE:ブルーススプリングスティーンの大ヒット曲 『Born in the USA』の歌詞の中で 『ベトナムに黄色い猿を殺しに行く』ってフレーズが あるんですけど、スプリングスティーンさんて 人種差別主...</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Source: カテゴリ一覧 - Yahoo!知恵袋Forum: 洋楽</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://detail.chiebukuro.yahoo.co.jp/qa/question_detail/q14227811489</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>コロナ給付金寄付プロジェクト「あなたの思いをあしたの支援に」検索IDでもっと便利に新規取得ログインお買い物がお得になるクーポンがたくさん条件指定質問・相談回答受付終了まであと4日　回答を投稿すると知恵コイン15枚が追加されますシェアツイートはてブ知恵コレID非公開さん2020/7/312:35:55ブルーススプリングスティーンの大ヒット曲
+『Born in the USA』の歌詞の中で
+『ベトナムに黄色い猿を殺しに行く』ってフレーズが
+あるんですけど、スプリングスティーンさんて人種差別主義者なんですか？違反報告回答投稿シェアツイートはてブ知恵コレ1〜5件/5件中猿メガネさん編集あり2020/7/517:01:15仮に黄色い猿と歌ってたとしても
+前後の文脈をしっかり聴けば
+人種差別主義者なんかでは
+ないことが理解できるはず。
+ある単語やフレーズだけを抜き出して
+過剰に反応する
+リテラシー能力のない人が
+最近は多いみたいやけど。違反報告kus********さん2020/7/319:45:27妄想が過ぎます違反報告不適切な内容が含まれている可能性があるため、非表示になっています。投稿内容に関する注意つぃんどっぐさん2020/7/314:41:04Got in a little hometown jam so they put rifle in my hand.
+Sent me off to a foriegan land to go and kill the yellow man.
+Born in the U.S.A.
+I was born in the U.S.A.
+.....
+どこにもyellow monkyとは書いてないが?違反報告質問者ID非公開さん2020/7/315:16:53Got in a little hometown jam
+So they put a rifle in my hand
+Sent me off to a foreign land
+To go and kill the yellow mon
+https://blog.goo.ne.jp/kantenbou/e/3bb6da51509f89f43922a62d2371fc7f
+書いてるじゃないか？違反報告その他の返信（2件）を表示ave********さん2020/7/312:48:03「黄色い猿」なんて歌っていません、「黄色い人間」の間違いです。
+人種をイエローというのは、そんなに差別的じゃないでしょう。違反報告一覧を見るみんなで作る知恵袋　悩みや疑問、なんでも気軽にきいちゃおう！Q&amp;Aをキーワードで検索：ランキングをもっと見る一覧を見るエンターテインメントと趣味∟音楽JASRAC許諾番号：9008249113Y38200Copyright (C) 2020 Yahoo Japan Corporation. All Rights Reserved.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Re: Anytown, USA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Source: The Motley Fool Discussion BoardsForum: Political Asylum</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://boards.fool.com/Message.aspx?mid=34552208&amp;sort=whole</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Folders | Best Of | Favorites &amp; Replies | Settings | Start a New Board | My Fool | Help |© 1995 - 2020 The Motley Fool. All rights reserved.
+Market data powered by FactSet and Web Financial Group.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>www.validdocumentsonline.com BUY REAL PASSPORTS / USA PASSPO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Source: AboutAlcoholismForum: Stories &amp; Journals</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>http://aboutalcoholism.proboards.com/post/5184/thread</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Welcome Guest. Please Login or Register.Welcome Guest. Please Login or Register.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>WTTF: Team USA Cards</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Source: Sports Card Trading and Sports Card ForumForum: Most Recent SCF Posts</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://www.sportscardforum.com/threads/2521884-WTTF-Team-USA-Cards</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>www.validdocumentsonline.com BUY REAL PASSPORTS / USA PASSPO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Source: Honda vt500 forumForum: Welcome</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>http://vt500-forum-uk.proboards.com/post/301/thread</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Welcome Guest. Please Login or Register.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RE:USA USA USA USA USA USA USA USA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Source: Where SRDines steal good drama from :)Forum: r/Drama</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Drama/comments/hl710m/usa_usa_usa_usa_usa_usa_usa_usa/fwxmmgr/</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>One more time for the commies in the backUSA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USAOne good thing to come out of this banwave stuff is that so many of these banned communities are making their own dedicated sites. Incels and T_D have had their sites for ages now, now you have radfems, femcels, and even cumboys going to their own sites/forums. Except of course chapos who have to once again prove to be a massive disappointment by going to that leftoid gab (raddle?) instead of making their own brand new site like everyone else. I imagine most of these sites are going to die out, but it would be nice if admins of massive sites kept going "NO FUN ALLOWED", leading to more and more communities bailing out and starting a forum renaissance.Oh yeah also thanks for reading my blog boys girls and everyone else.Actress and model Molly Conlin, 19, who starred in British soap opera EastEnders, claimed on Twitter that she was attacked in her home by a gang of "tall black men" who "barged in" and pinned her down on the ground as they robbed her.This image shows her original Twitter posts. Here's a Sun article reporting on her account of the incident.People soon noticed that Molly's social media was filled with seeming to support the BlackLivesMatter movement, demanding racial justice and attacking police as racist killers.https://www.reddithelp.com/en/categories/rules-reporting/account-and-community-restrictions/promoting-hate-based-identity-orThey removed the part saying majority groups are not protected from hate. Why can't we dunk on mayos in peace? Very bad for dramacoin. Smh.MembersOnline</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Paragraph</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>An American dream: Broadcasting AFL in the USA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>The Guardian</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.theguardian.com/sport/2020/jul/07/an-american-dream-broadcasting-afl-in-the-usa&amp;ct=ga&amp;cd=CAAYADIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNEZmUI53yb2cHlv3m53ZJFPA5n_2g</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>After the North American broadcast of the 1997 AFL grand final was delayed, a bunch of footy enthusiasts responded by buying the TV rightsJonathan HowcroftMon 6 Jul 2020 18.30 BST
+Last modified on Mon 6 Jul 2020E
+d Wyatt has the most interesting CV in Australian sport. As a TV host and radio commentator he has called or reported on it all, but fans of Australian basketball, baseball and football in particular will recognise his West Coast accent. Before that he won Emmys as a regular cast member of the sketch comedy show Almost Live! That was during his time in Seattle around the turn of the 1990s when the zeitgeist resided in the Pacific Northwest.In between those two lives Wyatt was part of a mob that bought the rights to broadcast the AFL in the USA, a story that includes the host of The Amazing Race, a star of Whose Line Is It Anyway, the brains behind BT Sport, and, most importantly of all, Wyatt’s wife, Michelle.With Australian sport bucking the global trend and providing some distraction from the pandemic there has been no shortage of attempts to recruit American viewers unfamiliar to Australian rules football. In light of this, the Wyatts recently revisited their own missionary project as part of The Greatest Season That Was podcast series.“It all came about because we wanted to watch the 1997 grand final between Adelaide and St Kilda on ESPN but the baseball that was on immediately beforehand went into extra innings, meaning the footy didn’t come on until midway through the opening quarter,” Wyatt explained to Guardian Australia. “No build-up, no anthems, and we were hosting a party at our place in Venice Beach, so we were furious.”In those days fury might have, at worst, led to a strongly worded letter to ESPN HQ, or the cancellation of a subscription, but the Wyatts were both employees of the recently launched Fox Sports World, giving them a platform to take more decisive action.Michelle Wyatt was a former producer of Channel Seven’s AFL coverage and the catalyst for the collective interest in the sport many miles from its heartland. Her Collingwood credentials go as far back as David Williamson’s seminal movie The Club where she appears in a crowd scene as a 12-year-old. She would later become the executive producer for Channel Ten’s popular series Before the Game.Michelle leveraged her contacts back in Australia to bring Fox Sports World into the conversation for securing AFL broadcast rights to avoid a repeat of the grand final debacle. Those negotiations were handled at the Los Angeles end by Simon Green who secured a three-year deal for one live game per week, one edited three-hour match, and one edited two-hour match. This was worth nothing to the AFL in year one, $40,000 in year two and $80,000 in year three. 15 years later Green was the driving force behind BT Sport shaking up coverage of the Premier League in the UK in a deal worth £246m per season.Fox Sports World only reached around 50,000 viewers by satellite, but the bigger carrot for the AFL was a route into America’s regional market under the umbrella of Fox Sports Net, where viewership jumped into the tens of millions. The campaign to grow subscribers mimicked the “I want my MTV” model of the 1980s with customers encouraged to call up their satellite provider at 1800 Fox World. Scripts to push this message via infomercials were written by Wyatt and voiced by Greg Proops and Phil Keoghan.After a near 20-year relationship with ESPN that had run out of steam, the AFL supported the new enterprise with priority access to players like Wayne Carey and James Hird, enabling the creation of a series of profiles and an A to Z of Australian rules primer. On trips back to Melbourne the Wyatts enjoyed an unfettered gameday experience, including the recording of links from the centre square of the MCG before the opening bounce. “Probably the most nervous I’ve ever been on television,” Wyatt recalls.The project peaked with the 1998 grand final. It was the first live broadcast accompanied by a dedicated pregame, hosted by Wyatt alongside the imported credentials of Gerard Healy. As part of the Fox Sports Net stable it was accessible in around 20 million homes.For all the ingenuity and talent involved the game didn’t take a quantum leap Stateside. Fox Sports World slashed its budget, while the obvious hook of Australian rules football to outsiders - the collisions and violence - was being legislated out of the game and downplayed for marketing purposes. But at least there was no longer baseball stopping play. “I think we delivered,” said Wyatt.The Wyatts relocated to Melbourne in 1999, mission somewhat accomplished. The AFL in the US has since gone full circle, first leaving Fox Sports World, spending a long time on the Setanta network, before eventually returning to Fox; still a niche offering, still with unrealised potential, still often viewed with mock-horror by disbelieving Americans wondering who forgot to bring the shoulder pads.“We were maybe ahead of our time,” Michelle Wyatt considers. With US networks still short of live sport to broadcast (turning recently to Adelaide v Fremantle as primetime fodder), and sports radio hosts clamouring for anything to get excited about, that groundwork may, belatedly, be coming to fruition.Hear more in The Greatest Season That Was Presents... we have a small favour to ask. Millions are flocking to the Guardian for quality news every day. We believe everyone deserves access to factual information, and analysis that has authority and integrity. That’s why, unlike many others, we made a choice: to keep Guardian reporting open for all, regardless of where they live or what they can afford to pay.As an open, independent news organisation we investigate, interrogate and expose the actions of those in power, without fear. With no shareholders or billionaire owner, our journalism is free from political and commercial bias – this makes us different. We can give a voice to the oppressed and neglected, and stand in solidarity with those who are calling for a fairer future. With your help we can make a difference.We’re determined to provide journalism that helps each of us better understand the world, and take actions that challenge, unite, and inspire change – in times of crisis and beyond. Our work would not be possible without our readers, who now support our work from 180 countries around the world.But news organisations are facing an existential threat. With advertising revenues plummeting, the Guardian risks losing a major source of its funding. More than ever before, we’re reliant on financial support from readers to fill the gap. Your support keeps us independent, open, and means we can maintain our high quality reporting – investigating, disentangling and interrogating.Every reader contribution, however big or small, is so valuable for our future. Support the Guardian from as little as $1 – and it only takes a minute. Thank you.Sign in or create your Guardian account to join the discussion.Given that the 1pm start games are 8PM starts on the west coast of the US, it is a shame that they are more often than not the lessor games of the round (Adelaide versus Freo being a prime example). Obviously broadcast considerations are always going to be dominated by Australian interests.Looking at the fixture, this Sunday's 1pm game is between Port and the Giants and next weeks Saturday 145 game is Giants v lions. Probably a quirk of having the three form teams in the comp being smaller clubs.14 comments in and half of them are from bitter Australian soccer fans....more comments than most articles on Australian soccer can musterImagine if their passionate hatred and jealousy at Australian football could be channelled positively into Australian soccer?We and our partners use your information – collected through cookies and similar technologies – to improve your experience on our site, analyse how you use it and show you personalised advertising.You can find out more in our privacy policy and cookie policy, and manage your consent at any time by going to ‘Privacy settings’ at the bottom of any page.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chris Moffett joins USA Groups</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Yahoo Finance</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/news/chris-moffett-joins-usa-groups-130000169.html&amp;ct=ga&amp;cd=CAAYATIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNF8y66blO66kc8vXVUw1QkFjkk34w</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SARASOTA, Fla., July 6, 2020 /PRNewswire/ -- Today, USA Groups, Inc. announced that Chris Moffett is joining the communications infrastructure firm as its new Chief Executive Officer. Moffett brings with him an extensive background in executive management, leadership, mergers and acquisitions, and strategic planning.  Moffett's knowledge of the communications industry will enable USA Groups to modify its unique product and service offerings."I could not be happier about bringing Chris into the USA Groups family.  For over 25 years the management team has positioned us as a leader in telecommunications construction and engineering by focusing on our customers' needs and then executing in a disciplined manner to consistently meet those needs," said James Goff, Executive Chairman (and now former CEO) of USA GROUPS.  "We are confident that Chris can accelerate our growth both organically and through strategic acquisitions.""I feel blessed to have been asked to lead USA Groups in its next phase of growth," stated
+Moffett.  "USA delivers a unique blend of products and services that are essential for the communications industry to deliver next generation networks.  USA Groups has a seasoned team of industry experts and I am excited to work with them to industrialize our offerings so that we can play an even larger role in helping our customers be successful."Moffett has 20 years of experience at Crown Castle International Corp. His prior roles included Director of International Acquisitions, Director of Commercial Strategy, Director of Finance and culminated with him being the President of Crown Castle's South Area for 14 years where he had P&amp;L responsibility for $1.3B in revenue, oversaw 11,000 macro sites, 20,000 small cell nodes and managed roughly 450 employees. Moffett holds a BSM in Finance and Marketing from Tulane University as well master's degrees in International Finance from The London School of Economics and Political Science as well as ASU's Thunderbird School of Global Management.About USA GROUPS
+USA GROUPS is a leading provider of construction, engineering and fabricated steel products to the telecommunications and infrastructure industries. These services, which are provided throughout the United States, include construction management, tower construction and modifications, engineering, structural steel fabrication, surveying, installation, and maintenance services to telecommunications providers, developers and government clients.  For more information on USA Groups, please visit www.usa-groups.com.Contact:
+Katie Kinnetz
+(800) 541-2170View original content to download multimedia:http://www.prnewswire.com/news-releases/chris-moffett-joins-usa-groups-301088331.htmlSOURCE USA Groups, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Coronavirus USA live updates: cases, deaths, news and stimulus checks, today, July 6th</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AS English</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://en.as.com/en/2020/07/06/latest_news/1593989092_414237.html&amp;ct=ga&amp;cd=CAAYAjIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNECgIKply8r6NwGfj08Yc25baXwBg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Latest NewsAS ENGLISHAccording to the latest figures published by John Hopkins University, 11,565,414 cases have been detected worldwide, with 536,650 deaths and 6,231,052 people recovered.In the USA, there have been 2,922,000 confirmed cases and 130,208 deaths, with 924,148 people recovered from the virus.It feels like, with Florida seeing a massive surge in cases, that this is not the best way to go about curbing the spread.Ventures backed by big-name entertainers Kanye West and Francis Ford Coppola were among those approved for loans under a U.S. government program to help businesses survive the coronavirus pandemic, according to a list released on Monday.Billionaire rapper West's clothing brand Yeezy received clearance for a loan of between $2 million and $5 million under the Paycheck Protection Program, the U.S. Small Business Administration said.The company said the loan would save 160 jobs, according to the SBA.The PPP was established to aid workers at companies and nonprofits with fewer than 500 employees hurt by closures and other measures meant to slow the spread of the novel coronavirus. The list released Monday gave the most-detailed accounting to date of who applied for and was approved to receive funds.US NEWSTrump Rallies for the 2020 presidential elections in the United States: schedule, dates and places42 states now seeing daily rises.Coronavirus has touched every aspect of American life. This US Covid-19 recovery hub will give you the data to measure where recovery is happening as it happens.With the news that there was a suspected case in China, questions were raised about what it could mean as we fight with the Covid-19 pandemic.CORONAVIRUSWhat is the bubonic plague, its symptoms and how it spreads?The Post looks at how Dr Fauci and others manage their lives amid the dangers of the current pandemic.In the span of a week and a half, the number of coronavirus cases in the United States has doubled, yet officials are saying this is still the first wave of the pandemic.Atlanta Mayor Keisha Lance Bottoms said on Monday that she has tested positive for Covid-19, but has not shown symptoms of the virus.She gave no information about her diagnosis, whether she is under quarantine and when she was tested. 'Covid-19 has literally hit home,' the first-term mayor of Georgia's state capital city said on Twitter.In New York, site of the country's largest outbreak, the state's curve rose sharply before reaching over 170,000 total cases in April. Since then, new cases have fallen from about 10,000 per day in mid-April to fewer than 700 per day in late June.Here are some of the stories that were making the headlines over the last 24 hours:- San Diego County was officially added to California's "monitoring list"- Sen. Grassley says he will skip Republican convention due to coronavirus concerns- MLB confirms testing delays, doesn't expect recurrence- Tiafoe out of World TeamTennis after positive test- Coronavirus hospitalizations grow in more than 20 states as Texas admissions soar to new record- Trump plans New Hampshire rally as he works to re-energize campaignAccording to the latest figures published by John Hopkins University, 11,565,414 cases have been detected worldwide, with 536,650 deaths and 6,231,052 people recovered.In the USA, there have been 2,922,000 confirmed cases and 130,208 deaths, with 924,148 people recovered from the virus.More than 11.5 million people globally have contracted the disease according to official figures, and well over half a million have lost their lives to the virus since it started to spread at the beginning of the year.In the US, the first wave was believed to be over but that is obviously not the case.Texas, Florida, Arizona and California have seen a resurgence in new cases and record numbers of hospitalisations reaffirming fears that a second wave, or a continuation of the first, is a very real possibility..0
+ComentariosEdiciones internacionalesAppsSíguenos© DIARIO AS, S.L. - Valentín Beato, 44 - 28037 Madrid [España] - Tel. 91 375 25 00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>'Grim resolve': Biden is up big and the Senate is in sight, but Democrats still haunted by fear of ...</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>USA TODAY</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.usatoday.com/story/news/politics/2020/07/05/joe-biden-up-big-and-senate-grasps-dems-haunted-fear-letdown/3284392001/&amp;ct=ga&amp;cd=CAAYBDIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNFVqXUXUEbGe2k2YcqJQm1uoXyndA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>WASHINGTON – Democrats have heard this story before.Their standard-bearer builds a sizable lead in the race for president against Donald Trump. Everything seems pointed in their direction. Pundits talk about a Democratic victory like it’s inevitable. Then it doesn’t happen.Still licking their wounds four years after Hillary Clinton’s stinging loss, Democrats are grappling with heightened expectations that didn’t seem possible at the start of the year. Presumptive Democratic nominee Joe Biden cruised to a double-digit lead nationally weeks ago and has stayed there as President Trump takes a pounding over his handling of the coronavirus crisis, high unemployment and the fallout from nationwide protests over police brutality.Not only does Biden lead polls in every battleground state – a wider command than Clinton ever had – the former vice president is either ahead or competitive in states that the GOP must carry, including Texas, Georgia, Iowa, Ohio and Missouri. Democrats also have a path to take control of the Senate.More:Trump trails Biden in Michigan, Wisconsin, Pennsylvania, Florida, North Carolina and Arizona, poll findsOn one hand, Democrats are gushing about their prospects: a chance for a sweeping victory, not just eking out a win, to deliver a clear repudiation of the Trump era and unseat Mitch McConnell as Senate majority leader.But they’re not able to shake off their painful memories of 2016, when many Democrats falsely assumed that the Republican Party’s nomination of a reality TV show host with no elected office experience would ensure a Clinton victory in November."That memory can't be erased," said Luis Heredia, executive director of the Arizona Education Association, the state's teachers union, and a Democratic National Committee member. He recalled watching swing states Pennsylvania and Michigan quickly collapse for Democrats on election night. “That memory is still very fresh, especially for me.”"You remind people that a poll is just a poll," Heredia said. "It's a moment in time on Tuesday morning when somebody answered a call. Let's not get carried away. We should be winning by 20 points, given the circumstances. Winning by 6 points is still too close for us to say that we're ahead of the game."In interviews with DNC members from six battleground states, including party leaders, each came back to an old campaign cliche: “Take nothing for granted.”Democratic anxiety is assuaged a bit by the different circumstances this time around: Trump is an incumbent, unable to run as a businessman outsider fighting to “drain the swamp.” Multiple crises – including a pandemic that’s resulted in more than 129,000 American deaths – are part of his record. He just wrapped up arguably the most difficult month in his presidency, capped by a controversy over reports that Russia offered bounties to the Taliban to kill U.S. soldiers.More:Trump denies knowing about intelligence report that Russia put bounty on US troops in AfghanistanPerhaps most significantly, Biden lacks the low favorability and trustworthiness marks that doomed Clinton, whose polarization gave Trump an opening many Democrats did not see.There is a major warning sign for Democrats: Despite Biden’s sizable lead, his supporters are significantly less enthusiastic about him than Trump’s loyalists are of the president, polling shows.“Democrats across Wisconsin have two reactions to this moment,” said Ben Wikler, chairman of the Wisconsin Democratic Party. “The first is that Trump is an unmitigated disaster, and polls demonstrate that everyone knows he’s bad. The second reaction is that we have learned our lesson from 2016.”He said Democrats “can’t take their foot off the gas even for a second” by buying too much into the polls, noting that Clinton led Trump by as many as 15 percentage points in Wisconsin after the Democratic National Convention in August 2016. Trump ended up winning Wisconsin by less than 1 percentage point.“I would encapsulate it as ‘grim resolve,’ ” Wikler said of the mood among Democrats. It’s “mystifying that Trump even has the scraps of support he has,” given his troubles. He said Democrats fear Trump is “willing to cheat his way back into power” by limiting voter access and refusing to accept results.More:Biden and Trump each warn that other side may 'steal' the election as fight over mail voting ragesThere are four months left before the election, enough time for the race to upend again.“The thing that keeps me up at night is the unknown unknowns,” Wikler said.Trump’s wins in Wisconsin, Michigan and Pennsylvania, three pivotal states that historically vote Democratic, proved fatal for Clinton in 2016. Winning back the Rust Belt is key for Biden, who holds a polling lead of 6 points or more in each state, according to the Real Clear Politics average of polls.Democratic leaders in these states said they began rebuilding campaign infrastructure quickly after their 2016 defeats in preparation for 2020.“I don’t think anybody is comfortable with these numbers,” said Lavora Barnes, chairwoman of the Michigan Democratic Party. “There were people in 2016 who, very early on, because of who Donald Trump was, thought, ‘How could this nation possibly choose Donald Trump?’ Now that that’s happened, we recognize that we should never count anybody out.”Barnes said the Clinton campaign started focusing on Michigan “late,” after the party conventions in the late summer, but the Biden campaign is already working closely with the state party’s operations.“We all recognize the importance of this moment and the opportunities here, but they are only opportunities for us if we take advantage of them by doing the work,” she said.Rick Bloomingdale, president of the Pennsylvania AFL-CIO and a DNC committee member, said Biden’s strong numbers show that workers are worried about the economy and the pandemic, and “they’re seeing no leadership from Washington, D.C.”“But that doesn't mean they're going to hold. Trump has shown an incredible ability to be down and then back up. A lot can happen in those (final 120) days. In 2016, people thought, 'Oh man, if they nominate Trump, this thing's a waltz.' It wasn't, of course. We shouldn't assume it's going to be this time."He said, "We'd all love for the election to be over today. But we also know that's not the case.”Asked whether he feels good about Biden carrying Pennsylvania, Bloomingdale said, “I was confident that Hillary was going to win Pennsylvania. If we do the work, we’ll win. If we don’t do the work, we won’t win.”Wikler said Democrats in Wisconsin “erased” the advantage an incumbent typically has by laying groundwork since 2017.Like Michigan and Pennsylvania, Trump carried Wisconsin with strong support from white, working-class voters, winning rural counties across the state with more than 60% of the vote. Since then, Wikler noted, Sen. Tammy Baldwin, D-Wis., won her reelection in 2018 by double digits. Wikler said he believes Biden can make more inroads in rural areas where farms have been hurt by Trump’s trade policies.“We know that Trump is targeting Wisconsin as an absolute-must state for reelection,” Wikler said. “For us, that means we have to fight for every vote, and we’re investing accordingly.”Biden leads Trump nationally, 53%-41%, according to a USA TODAY/Suffolk University poll released last week, and holds a 9.4% lead in the Real Clear Politics average of polls.At this juncture in 2016, Clinton’s advantage over Trump was smaller, 46%-40% in the USATODAY/Suffolk poll, and Trump started to close the gap. In the Real Clear Politics average of polls on July 1, 2016, Clinton led by 4.8 points, a tightening from her double-digit advantage in the spring.Exclusive USA TODAY poll: Biden widens his lead, but Trump keeps the edge on enthusiasmAlthough some slammed the accuracy of polling after Trump won in an upset, Clinton's final lead in the popular vote, 48.2% to 46.1%, closely matched final polls. Trump's edge in the Electoral College came from close wins in swing states.Troubling for Trump this go-around: Only 20% of voters surveyed in the USA TODAY poll say the USA is headed in the right direction. The majority (67%) say the country is headed in the wrong direction. Biden also lacks the same negatives as Clinton, including questions over character.Fifty percent of voters surveyed say they find Biden honest and trustworthy, compared with 30% for Trump. Six weeks before the 2016 election, Trump led the trustworthy question. A Washington Post/ABC poll found 33% of voters found Clinton honest and trustworthy, and Trump was trusted by 42%.David Paleologos, director of Suffolk University’s Political Research Center, said the 2016 electorate was swung by “the haters” – voters who disliked both Trump and Clinton. He said the “intensity against Hillary Clinton ended up being higher than Trump, especially in the swing states.” Trump benefited by a race that turned highly negative because Clinton was more polarizing. “This year, you don’t have that,” Paleologos said. “He’s likable. He’s likable Joe.”Paleologos on the poll: First, we couldn't talk politics at Thanksgiving. Now, the 4th?For Trump, Paleologos said, “that’s really the challenge ahead. He doesn’t have an opponent who people hate or have a visceral reaction to.”Biden’s biggest vulnerability could be the enthusiasm gap. Most of his supporters back him because he’s “not Trump,” according to Paleologos. Half of Trump's backers say they are "very excited" about their candidate; 27% of Biden backers say that. “The people for Trump, they love him. The people for Biden, they shrug their shoulders,” Paleologos said.Biden leads overwhelmingly among voters not enthusiastic about either candidate. “That’s right now taking its toll on the Trump campaign,” Paleologos said.Biden downplayed his lead during his first news conference since April after a speech last week in Wilmington, Delaware. He was asked about his unorthodox campaign, which has operated largely from his home in Delaware during the pandemic. Biden said “the irony” is he’s probably been able to reach more voters through virtual campaigning.“So far, it remains to be seen, I don’t want to jinx myself, I know the polling data is very good. But I think it’s really early. It’s much too early to make any judgment,” Biden said.Biden in the basement: Can campaigning from home work as Trump starts to travel?Trump and Republicans have struggled to find an attack against Biden that’s stuck.During a conference call with reporters, Trump communication director Tim Murtaugh threw the gauntlet at Biden.He slammed Biden for not denouncing the tear-downs of monuments by protesters, called him a “disaster” on the economy, talked extensively about Rep. Alexandria Ocasio-Cortez, D-N.Y., questioned Biden’s ties to China and argued the Obama-Biden administration’s handling of the H1N1 pandemic left Trump with a shortage of N95 masks. He accused Biden of using COVID-19 as a “political weapon in a cynical attempt” to undermine public confidence.“Joe Biden is hoping to ride out the rest of these four months without taking any of these questions,” Murtaugh said. “He’s not undergoing thorough vetting before the American people, and he’s not facing scrutiny because his handlers know he is not up to it.”Comparing the 2020 and 2016 elections, Robby Mook, Clinton's 2016 campaign manager, said last week, “I almost look at it as: Is there very much that’s the same?” He appeared on the podcast of David Plouffe, Barack Obama’s former campaign manager. “First and foremost, I’d say COVID has changed everything.”Mook, president of the House Majority PAC, said Trump is taken "more seriously" and "being held to account in a way that he wasn’t in ’16.” Whereas Trump’s "petty" remarks were treated as a “novelty” in 2016, they’re now seen “in a context of a true lack of leadership,” he said. Political experience tends to be a liability in campaigns, Mook said, but it’s viewed as a strength for Biden during the pandemic. “I think Hillary kind of got the opposite end of that." He predicted the race would tighten up as voters, as they historically do, "go home to their parties," but not if Trump can't "get his act together."“Biden wants this to be a referendum on Trump, and he’s winning that right now. Trump needs to reengineer that to be a choice – and he can’t even offer what that choice is," Mook said. "So how in the world are they supposed to get this on firmer ground for their strategy?”None of the Trump taglines on Biden has gained traction like “Crooked Hillary” and chants of “Lock her up” four years ago.Democrats, despite their cautious optimism, are bullish about the issues being in their favor: a pandemic they contend exposed failed presidential leadership and Trump's “law and order” response to protests over systemic racism and police brutality as polling shows more Americans are favorable to the Black Lives Matter movement. "We understand what the temperature and the pulse of the country looks like right now,” said Shelia Huggins, an attorney from Durham, North Carolina, and DNC committee member.More:Joe Biden campaign seizes on opportunity to contrast Trump's 'law and order' messageShe said her Democratic friends aren’t talking about a 2016 repeat as much as they once were."We’re too busy listening to a president who is talking nonsense pretty much every day,” she said. “You're easily reminded that 2016 is not what needs to be on the forefront of what we're thinking about. We need to be thinking about 2020."In Arizona, Heredia said he believes Democrats have momentum to carry the state for Biden, win the U.S. Senate race between Democrat Mark Kelly and Sen. Martha McSally and flip both chambers of the state Legislature, where Republicans have slim majorities. The last Democrat to carry Arizona for president was Bill Clinton in 1996. “There's a perfect storm building up in Arizona, I would call it a perfect ‘haboob’ in our state,” he said, referring to the dust storms that pop up in the SouthwestMore:Trump calls proposed Black Lives Matter mural outside Trump Tower 'a symbol of hate'Ken Evans, a DNC committee member from Florida, who runs a camp for children in Fort Lauderdale, said he knows many "nonpartisan people" in Broward County who voted for Trump because they couldn’t back Clinton, but they plan to vote for Biden in November. He said the president’s handling of the coronavirus was the last straw.“That’s making the difference. That’s what’s going to bring out the vote,” Evans said, defending voter enthusiasm for Biden. “They’re excited to bring normalcy back to the White House” after all the "tiresome" Trump drama, he said. “People are tired.”When it comes to Biden being ahead in polls, though, Evans returned to four years ago.“So was Hillary, right?” he said.Reach Joey Garrison on Twitter @joeygarrison.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RE:ブルーススプリングスティーンの大ヒット曲 『Born in the USA』の歌詞の中で 『ベトナムに黄色い猿を殺しに行く』ってフレーズが あるんですけど、スプリングスティーンさんて 人種差別主...</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Source: カテゴリ一覧 - Yahoo!知恵袋Forum: 洋楽</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://detail.chiebukuro.yahoo.co.jp/qa/question_detail/q14227811489</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>コロナ給付金寄付プロジェクト「あなたの思いをあしたの支援に」検索IDでもっと便利に新規取得ログインお買い物がお得になるクーポンがたくさん条件指定質問・相談回答受付終了まであと4日　回答を投稿すると知恵コイン15枚が追加されますシェアツイートはてブ知恵コレID非公開さん2020/7/312:35:55ブルーススプリングスティーンの大ヒット曲
+『Born in the USA』の歌詞の中で
+『ベトナムに黄色い猿を殺しに行く』ってフレーズが
+あるんですけど、スプリングスティーンさんて人種差別主義者なんですか？違反報告回答投稿シェアツイートはてブ知恵コレ1〜5件/5件中猿メガネさん編集あり2020/7/517:01:15仮に黄色い猿と歌ってたとしても
+前後の文脈をしっかり聴けば
+人種差別主義者なんかでは
+ないことが理解できるはず。
+ある単語やフレーズだけを抜き出して
+過剰に反応する
+リテラシー能力のない人が
+最近は多いみたいやけど。違反報告kus********さん2020/7/319:45:27妄想が過ぎます違反報告不適切な内容が含まれている可能性があるため、非表示になっています。投稿内容に関する注意つぃんどっぐさん2020/7/314:41:04Got in a little hometown jam so they put rifle in my hand.
+Sent me off to a foriegan land to go and kill the yellow man.
+Born in the U.S.A.
+I was born in the U.S.A.
+.....
+どこにもyellow monkyとは書いてないが?違反報告質問者ID非公開さん2020/7/315:16:53Got in a little hometown jam
+So they put a rifle in my hand
+Sent me off to a foreign land
+To go and kill the yellow mon
+https://blog.goo.ne.jp/kantenbou/e/3bb6da51509f89f43922a62d2371fc7f
+書いてるじゃないか？違反報告その他の返信（3件）を表示ave********さん2020/7/312:48:03「黄色い猿」なんて歌っていません、「黄色い人間」の間違いです。
+人種をイエローというのは、そんなに差別的じゃないでしょう。違反報告一覧を見るみんなで作る知恵袋　悩みや疑問、なんでも気軽にきいちゃおう！Q&amp;Aをキーワードで検索：ランキングをもっと見る一覧を見るエンターテインメントと趣味∟音楽JASRAC許諾番号：9008249113Y38200Copyright (C) 2020 Yahoo Japan Corporation. All Rights Reserved.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Re: Anytown, USA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Source: The Motley Fool Discussion BoardsForum: Political Asylum</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://boards.fool.com/Message.aspx?mid=34552208&amp;sort=whole</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Folders | Best Of | Favorites &amp; Replies | Settings | Start a New Board | My Fool | Help |© 1995 - 2020 The Motley Fool. All rights reserved.
+Market data powered by FactSet and Web Financial Group.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>www.validdocumentsonline.com BUY REAL PASSPORTS / USA PASSPO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Source: AboutAlcoholismForum: Stories &amp; Journals</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>http://aboutalcoholism.proboards.com/post/5184/thread</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Welcome Guest. Please Login or Register.Welcome Guest. Please Login or Register.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>WTTF: Team USA Cards</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Source: Sports Card Trading and Sports Card ForumForum: Most Recent SCF Posts</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://www.sportscardforum.com/threads/2521884-WTTF-Team-USA-Cards</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>www.validdocumentsonline.com BUY REAL PASSPORTS / USA PASSPO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Source: Honda vt500 forumForum: Welcome</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>http://vt500-forum-uk.proboards.com/post/301/thread</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Welcome Guest. Please Login or Register.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RE:USA USA USA USA USA USA USA USA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Source: Where SRDines steal good drama from :)Forum: r/Drama</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Drama/comments/hl710m/usa_usa_usa_usa_usa_usa_usa_usa/fwxmmgr/</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>One more time for the commies in the backUSA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USA USAMembersOnline</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Paragraph</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>An American dream: Broadcasting AFL in the USA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>The Guardian</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.theguardian.com/sport/2020/jul/07/an-american-dream-broadcasting-afl-in-the-usa&amp;ct=ga&amp;cd=CAAYADIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNEZmUI53yb2cHlv3m53ZJFPA5n_2g</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>After the North American broadcast of the 1997 AFL grand final was delayed, a bunch of footy enthusiasts responded by buying the TV rightsJonathan HowcroftMon 6 Jul 2020 18.30 BST
+Last modified on Mon 6 Jul 2020E
+d Wyatt has the most interesting CV in Australian sport. As a TV host and radio commentator he has called or reported on it all, but fans of Australian basketball, baseball and football in particular will recognise his West Coast accent. Before that he won Emmys as a regular cast member of the sketch comedy show Almost Live! That was during his time in Seattle around the turn of the 1990s when the zeitgeist resided in the Pacific Northwest.In between those two lives Wyatt was part of a mob that bought the rights to broadcast the AFL in the USA, a story that includes the host of The Amazing Race, a star of Whose Line Is It Anyway, the brains behind BT Sport, and, most importantly of all, Wyatt’s wife, Michelle.With Australian sport bucking the global trend and providing some distraction from the pandemic there has been no shortage of attempts to recruit American viewers unfamiliar to Australian rules football. In light of this, the Wyatts recently revisited their own missionary project as part of The Greatest Season That Was podcast series.“It all came about because we wanted to watch the 1997 grand final between Adelaide and St Kilda on ESPN but the baseball that was on immediately beforehand went into extra innings, meaning the footy didn’t come on until midway through the opening quarter,” Wyatt explained to Guardian Australia. “No build-up, no anthems, and we were hosting a party at our place in Venice Beach, so we were furious.”In those days fury might have, at worst, led to a strongly worded letter to ESPN HQ, or the cancellation of a subscription, but the Wyatts were both employees of the recently launched Fox Sports World, giving them a platform to take more decisive action.Michelle Wyatt was a former producer of Channel Seven’s AFL coverage and the catalyst for the collective interest in the sport many miles from its heartland. Her Collingwood credentials go as far back as David Williamson’s seminal movie The Club where she appears in a crowd scene as a 12-year-old. She would later become the executive producer for Channel Ten’s popular series Before the Game.Michelle leveraged her contacts back in Australia to bring Fox Sports World into the conversation for securing AFL broadcast rights to avoid a repeat of the grand final debacle. Those negotiations were handled at the Los Angeles end by Simon Green who secured a three-year deal for one live game per week, one edited three-hour match, and one edited two-hour match. This was worth nothing to the AFL in year one, $40,000 in year two and $80,000 in year three. 15 years later Green was the driving force behind BT Sport shaking up coverage of the Premier League in the UK in a deal worth £246m per season.Fox Sports World only reached around 50,000 viewers by satellite, but the bigger carrot for the AFL was a route into America’s regional market under the umbrella of Fox Sports Net, where viewership jumped into the tens of millions. The campaign to grow subscribers mimicked the “I want my MTV” model of the 1980s with customers encouraged to call up their satellite provider at 1800 Fox World. Scripts to push this message via infomercials were written by Wyatt and voiced by Greg Proops and Phil Keoghan.After a near 20-year relationship with ESPN that had run out of steam, the AFL supported the new enterprise with priority access to players like Wayne Carey and James Hird, enabling the creation of a series of profiles and an A to Z of Australian rules primer. On trips back to Melbourne the Wyatts enjoyed an unfettered gameday experience, including the recording of links from the centre square of the MCG before the opening bounce. “Probably the most nervous I’ve ever been on television,” Wyatt recalls.The project peaked with the 1998 grand final. It was the first live broadcast accompanied by a dedicated pregame, hosted by Wyatt alongside the imported credentials of Gerard Healy. As part of the Fox Sports Net stable it was accessible in around 20 million homes.For all the ingenuity and talent involved the game didn’t take a quantum leap Stateside. Fox Sports World slashed its budget, while the obvious hook of Australian rules football to outsiders - the collisions and violence - was being legislated out of the game and downplayed for marketing purposes. But at least there was no longer baseball stopping play. “I think we delivered,” said Wyatt.The Wyatts relocated to Melbourne in 1999, mission somewhat accomplished. The AFL in the US has since gone full circle, first leaving Fox Sports World, spending a long time on the Setanta network, before eventually returning to Fox; still a niche offering, still with unrealised potential, still often viewed with mock-horror by disbelieving Americans wondering who forgot to bring the shoulder pads.“We were maybe ahead of our time,” Michelle Wyatt considers. With US networks still short of live sport to broadcast (turning recently to Adelaide v Fremantle as primetime fodder), and sports radio hosts clamouring for anything to get excited about, that groundwork may, belatedly, be coming to fruition.Hear more in The Greatest Season That Was Presents... we have a small favour to ask. Millions are flocking to the Guardian for quality news every day. We believe everyone deserves access to factual information, and analysis that has authority and integrity. That’s why, unlike many others, we made a choice: to keep Guardian reporting open for all, regardless of where they live or what they can afford to pay.As an open, independent news organisation we investigate, interrogate and expose the actions of those in power, without fear. With no shareholders or billionaire owner, our journalism is free from political and commercial bias – this makes us different. We can give a voice to the oppressed and neglected, and stand in solidarity with those who are calling for a fairer future. With your help we can make a difference.We’re determined to provide journalism that helps each of us better understand the world, and take actions that challenge, unite, and inspire change – in times of crisis and beyond. Our work would not be possible without our readers, who now support our work from 180 countries around the world.But news organisations are facing an existential threat. With advertising revenues plummeting, the Guardian risks losing a major source of its funding. More than ever before, we’re reliant on financial support from readers to fill the gap. Your support keeps us independent, open, and means we can maintain our high quality reporting – investigating, disentangling and interrogating.Every reader contribution, however big or small, is so valuable for our future. Support the Guardian from as little as $1 – and it only takes a minute. Thank you.Sign in or create your Guardian account to join the discussion.Given that the 1pm start games are 8PM starts on the west coast of the US, it is a shame that they are more often than not the lessor games of the round (Adelaide versus Freo being a prime example). Obviously broadcast considerations are always going to be dominated by Australian interests.Looking at the fixture, this Sunday's 1pm game is between Port and the Giants and next weeks Saturday 145 game is Giants v lions. Probably a quirk of having the three form teams in the comp being smaller clubs.14 comments in and half of them are from bitter Australian soccer fans....more comments than most articles on Australian soccer can musterImagine if their passionate hatred and jealousy at Australian football could be channelled positively into Australian soccer?We and our partners use your information – collected through cookies and similar technologies – to improve your experience on our site, analyse how you use it and show you personalised advertising.You can find out more in our privacy policy and cookie policy, and manage your consent at any time by going to ‘Privacy settings’ at the bottom of any page.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chris Moffett joins USA Groups</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Yahoo Finance</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/news/chris-moffett-joins-usa-groups-130000169.html&amp;ct=ga&amp;cd=CAAYATIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNF8y66blO66kc8vXVUw1QkFjkk34w</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SARASOTA, Fla., July 6, 2020 /PRNewswire/ -- Today, USA Groups, Inc. announced that Chris Moffett is joining the communications infrastructure firm as its new Chief Executive Officer. Moffett brings with him an extensive background in executive management, leadership, mergers and acquisitions, and strategic planning.  Moffett's knowledge of the communications industry will enable USA Groups to modify its unique product and service offerings."I could not be happier about bringing Chris into the USA Groups family.  For over 25 years the management team has positioned us as a leader in telecommunications construction and engineering by focusing on our customers' needs and then executing in a disciplined manner to consistently meet those needs," said James Goff, Executive Chairman (and now former CEO) of USA GROUPS.  "We are confident that Chris can accelerate our growth both organically and through strategic acquisitions.""I feel blessed to have been asked to lead USA Groups in its next phase of growth," stated
+Moffett.  "USA delivers a unique blend of products and services that are essential for the communications industry to deliver next generation networks.  USA Groups has a seasoned team of industry experts and I am excited to work with them to industrialize our offerings so that we can play an even larger role in helping our customers be successful."Moffett has 20 years of experience at Crown Castle International Corp. His prior roles included Director of International Acquisitions, Director of Commercial Strategy, Director of Finance and culminated with him being the President of Crown Castle's South Area for 14 years where he had P&amp;L responsibility for $1.3B in revenue, oversaw 11,000 macro sites, 20,000 small cell nodes and managed roughly 450 employees. Moffett holds a BSM in Finance and Marketing from Tulane University as well master's degrees in International Finance from The London School of Economics and Political Science as well as ASU's Thunderbird School of Global Management.About USA GROUPS
+USA GROUPS is a leading provider of construction, engineering and fabricated steel products to the telecommunications and infrastructure industries. These services, which are provided throughout the United States, include construction management, tower construction and modifications, engineering, structural steel fabrication, surveying, installation, and maintenance services to telecommunications providers, developers and government clients.  For more information on USA Groups, please visit www.usa-groups.com.Contact:
+Katie Kinnetz
+(800) 541-2170View original content to download multimedia:http://www.prnewswire.com/news-releases/chris-moffett-joins-usa-groups-301088331.htmlSOURCE USA Groups, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Coronavirus USA live updates: cases, deaths, news and stimulus checks, today, July 6th</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AS English</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://en.as.com/en/2020/07/06/latest_news/1593989092_414237.html&amp;ct=ga&amp;cd=CAAYAjIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNECgIKply8r6NwGfj08Yc25baXwBg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Latest NewsAS ENGLISHAccording to the latest figures published by John Hopkins University, 11,565,414 cases have been detected worldwide, with 536,650 deaths and 6,231,052 people recovered.In the USA, there have been 2,922,000 confirmed cases and 130,208 deaths, with 924,148 people recovered from the virus.It feels like, with Florida seeing a massive surge in cases, that this is not the best way to go about curbing the spread.Ventures backed by big-name entertainers Kanye West and Francis Ford Coppola were among those approved for loans under a U.S. government program to help businesses survive the coronavirus pandemic, according to a list released on Monday.Billionaire rapper West's clothing brand Yeezy received clearance for a loan of between $2 million and $5 million under the Paycheck Protection Program, the U.S. Small Business Administration said.The company said the loan would save 160 jobs, according to the SBA.The PPP was established to aid workers at companies and nonprofits with fewer than 500 employees hurt by closures and other measures meant to slow the spread of the novel coronavirus. The list released Monday gave the most-detailed accounting to date of who applied for and was approved to receive funds.US NEWSTrump Rallies for the 2020 presidential elections in the United States: schedule, dates and places42 states now seeing daily rises.Coronavirus has touched every aspect of American life. This US Covid-19 recovery hub will give you the data to measure where recovery is happening as it happens.With the news that there was a suspected case in China, questions were raised about what it could mean as we fight with the Covid-19 pandemic.CORONAVIRUSWhat is the bubonic plague, its symptoms and how it spreads?The Post looks at how Dr Fauci and others manage their lives amid the dangers of the current pandemic.In the span of a week and a half, the number of coronavirus cases in the United States has doubled, yet officials are saying this is still the first wave of the pandemic.Atlanta Mayor Keisha Lance Bottoms said on Monday that she has tested positive for Covid-19, but has not shown symptoms of the virus.She gave no information about her diagnosis, whether she is under quarantine and when she was tested. 'Covid-19 has literally hit home,' the first-term mayor of Georgia's state capital city said on Twitter.In New York, site of the country's largest outbreak, the state's curve rose sharply before reaching over 170,000 total cases in April. Since then, new cases have fallen from about 10,000 per day in mid-April to fewer than 700 per day in late June.Here are some of the stories that were making the headlines over the last 24 hours:- San Diego County was officially added to California's "monitoring list"- Sen. Grassley says he will skip Republican convention due to coronavirus concerns- MLB confirms testing delays, doesn't expect recurrence- Tiafoe out of World TeamTennis after positive test- Coronavirus hospitalizations grow in more than 20 states as Texas admissions soar to new record- Trump plans New Hampshire rally as he works to re-energize campaignAccording to the latest figures published by John Hopkins University, 11,565,414 cases have been detected worldwide, with 536,650 deaths and 6,231,052 people recovered.In the USA, there have been 2,922,000 confirmed cases and 130,208 deaths, with 924,148 people recovered from the virus.More than 11.5 million people globally have contracted the disease according to official figures, and well over half a million have lost their lives to the virus since it started to spread at the beginning of the year.In the US, the first wave was believed to be over but that is obviously not the case.Texas, Florida, Arizona and California have seen a resurgence in new cases and record numbers of hospitalisations reaffirming fears that a second wave, or a continuation of the first, is a very real possibility..0
+ComentariosEdiciones internacionalesAppsSíguenos© DIARIO AS, S.L. - Valentín Beato, 44 - 28037 Madrid [España] - Tel. 91 375 25 00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>'Grim resolve': Biden is up big and the Senate is in sight, but Democrats still haunted by fear of ...</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>USA TODAY</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.usatoday.com/story/news/politics/2020/07/05/joe-biden-up-big-and-senate-grasps-dems-haunted-fear-letdown/3284392001/&amp;ct=ga&amp;cd=CAAYBDIdYzdhYjFmODVkNmQ0NWMzNDpjb20uc2c6ZW46U0c&amp;usg=AFQjCNFVqXUXUEbGe2k2YcqJQm1uoXyndA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>WASHINGTON – Democrats have heard this story before.Their standard-bearer builds a sizable lead in the race for president against Donald Trump. Everything seems pointed in their direction. Pundits talk about a Democratic victory like it’s inevitable. Then it doesn’t happen.Still licking their wounds four years after Hillary Clinton’s stinging loss, Democrats are grappling with heightened expectations that didn’t seem possible at the start of the year. Presumptive Democratic nominee Joe Biden cruised to a double-digit lead nationally weeks ago and has stayed there as President Trump takes a pounding over his handling of the coronavirus crisis, high unemployment and the fallout from nationwide protests over police brutality.Not only does Biden lead polls in every battleground state – a wider command than Clinton ever had – the former vice president is either ahead or competitive in states that the GOP must carry, including Texas, Georgia, Iowa, Ohio and Missouri. Democrats also have a path to take control of the Senate.More:Trump trails Biden in Michigan, Wisconsin, Pennsylvania, Florida, North Carolina and Arizona, poll findsOn one hand, Democrats are gushing about their prospects: a chance for a sweeping victory, not just eking out a win, to deliver a clear repudiation of the Trump era and unseat Mitch McConnell as Senate majority leader.But they’re not able to shake off their painful memories of 2016, when many Democrats falsely assumed that the Republican Party’s nomination of a reality TV show host with no elected office experience would ensure a Clinton victory in November."That memory can't be erased," said Luis Heredia, executive director of the Arizona Education Association, the state's teachers union, and a Democratic National Committee member. He recalled watching swing states Pennsylvania and Michigan quickly collapse for Democrats on election night. “That memory is still very fresh, especially for me.”"You remind people that a poll is just a poll," Heredia said. "It's a moment in time on Tuesday morning when somebody answered a call. Let's not get carried away. We should be winning by 20 points, given the circumstances. Winning by 6 points is still too close for us to say that we're ahead of the game."In interviews with DNC members from six battleground states, including party leaders, each came back to an old campaign cliche: “Take nothing for granted.”Democratic anxiety is assuaged a bit by the different circumstances this time around: Trump is an incumbent, unable to run as a businessman outsider fighting to “drain the swamp.” Multiple crises – including a pandemic that’s resulted in more than 129,000 American deaths – are part of his record. He just wrapped up arguably the most difficult month in his presidency, capped by a controversy over reports that Russia offered bounties to the Taliban to kill U.S. soldiers.More:Trump denies knowing about intelligence report that Russia put bounty on US troops in AfghanistanPerhaps most significantly, Biden lacks the low favorability and trustworthiness marks that doomed Clinton, whose polarization gave Trump an opening many Democrats did not see.There is a major warning sign for Democrats: Despite Biden’s sizable lead, his supporters are significantly less enthusiastic about him than Trump’s loyalists are of the president, polling shows.“Democrats across Wisconsin have two reactions to this moment,” said Ben Wikler, chairman of the Wisconsin Democratic Party. “The first is that Trump is an unmitigated disaster, and polls demonstrate that everyone knows he’s bad. The second reaction is that we have learned our lesson from 2016.”He said Democrats “can’t take their foot off the gas even for a second” by buying too much into the polls, noting that Clinton led Trump by as many as 15 percentage points in Wisconsin after the Democratic National Convention in August 2016. Trump ended up winning Wisconsin by less than 1 percentage point.“I would encapsulate it as ‘grim resolve,’ ” Wikler said of the mood among Democrats. It’s “mystifying that Trump even has the scraps of support he has,” given his troubles. He said Democrats fear Trump is “willing to cheat his way back into power” by limiting voter access and refusing to accept results.More:Biden and Trump each warn that other side may 'steal' the election as fight over mail voting ragesThere are four months left before the election, enough time for the race to upend again.“The thing that keeps me up at night is the unknown unknowns,” Wikler said.Trump’s wins in Wisconsin, Michigan and Pennsylvania, three pivotal states that historically vote Democratic, proved fatal for Clinton in 2016. Winning back the Rust Belt is key for Biden, who holds a polling lead of 6 points or more in each state, according to the Real Clear Politics average of polls.Democratic leaders in these states said they began rebuilding campaign infrastructure quickly after their 2016 defeats in preparation for 2020.“I don’t think anybody is comfortable with these numbers,” said Lavora Barnes, chairwoman of the Michigan Democratic Party. “There were people in 2016 who, very early on, because of who Donald Trump was, thought, ‘How could this nation possibly choose Donald Trump?’ Now that that’s happened, we recognize that we should never count anybody out.”Barnes said the Clinton campaign started focusing on Michigan “late,” after the party conventions in the late summer, but the Biden campaign is already working closely with the state party’s operations.“We all recognize the importance of this moment and the opportunities here, but they are only opportunities for us if we take advantage of them by doing the work,” she said.Rick Bloomingdale, president of the Pennsylvania AFL-CIO and a DNC committee member, said Biden’s strong numbers show that workers are worried about the economy and the pandemic, and “they’re seeing no leadership from Washington, D.C.”“But that doesn't mean they're going to hold. Trump has shown an incredible ability to be down and then back up. A lot can happen in those (final 120) days. In 2016, people thought, 'Oh man, if they nominate Trump, this thing's a waltz.' It wasn't, of course. We shouldn't assume it's going to be this time."He said, "We'd all love for the election to be over today. But we also know that's not the case.”Asked whether he feels good about Biden carrying Pennsylvania, Bloomingdale said, “I was confident that Hillary was going to win Pennsylvania. If we do the work, we’ll win. If we don’t do the work, we won’t win.”Wikler said Democrats in Wisconsin “erased” the advantage an incumbent typically has by laying groundwork since 2017.Like Michigan and Pennsylvania, Trump carried Wisconsin with strong support from white, working-class voters, winning rural counties across the state with more than 60% of the vote. Since then, Wikler noted, Sen. Tammy Baldwin, D-Wis., won her reelection in 2018 by double digits. Wikler said he believes Biden can make more inroads in rural areas where farms have been hurt by Trump’s trade policies.“We know that Trump is targeting Wisconsin as an absolute-must state for reelection,” Wikler said. “For us, that means we have to fight for every vote, and we’re investing accordingly.”Biden leads Trump nationally, 53%-41%, according to a USA TODAY/Suffolk University poll released last week, and holds a 9.4% lead in the Real Clear Politics average of polls.At this juncture in 2016, Clinton’s advantage over Trump was smaller, 46%-40% in the USATODAY/Suffolk poll, and Trump started to close the gap. In the Real Clear Politics average of polls on July 1, 2016, Clinton led by 4.8 points, a tightening from her double-digit advantage in the spring.Exclusive USA TODAY poll: Biden widens his lead, but Trump keeps the edge on enthusiasmAlthough some slammed the accuracy of polling after Trump won in an upset, Clinton's final lead in the popular vote, 48.2% to 46.1%, closely matched final polls. Trump's edge in the Electoral College came from close wins in swing states.Troubling for Trump this go-around: Only 20% of voters surveyed in the USA TODAY poll say the USA is headed in the right direction. The majority (67%) say the country is headed in the wrong direction. Biden also lacks the same negatives as Clinton, including questions over character.Fifty percent of voters surveyed say they find Biden honest and trustworthy, compared with 30% for Trump. Six weeks before the 2016 election, Trump led the trustworthy question. A Washington Post/ABC poll found 33% of voters found Clinton honest and trustworthy, and Trump was trusted by 42%.David Paleologos, director of Suffolk University’s Political Research Center, said the 2016 electorate was swung by “the haters” – voters who disliked both Trump and Clinton. He said the “intensity against Hillary Clinton ended up being higher than Trump, especially in the swing states.” Trump benefited by a race that turned highly negative because Clinton was more polarizing. “This year, you don’t have that,” Paleologos said. “He’s likable. He’s likable Joe.”Paleologos on the poll: First, we couldn't talk politics at Thanksgiving. Now, the 4th?For Trump, Paleologos said, “that’s really the challenge ahead. He doesn’t have an opponent who people hate or have a visceral reaction to.”Biden’s biggest vulnerability could be the enthusiasm gap. Most of his supporters back him because he’s “not Trump,” according to Paleologos. Half of Trump's backers say they are "very excited" about their candidate; 27% of Biden backers say that. “The people for Trump, they love him. The people for Biden, they shrug their shoulders,” Paleologos said.Biden leads overwhelmingly among voters not enthusiastic about either candidate. “That’s right now taking its toll on the Trump campaign,” Paleologos said.Biden downplayed his lead during his first news conference since April after a speech last week in Wilmington, Delaware. He was asked about his unorthodox campaign, which has operated largely from his home in Delaware during the pandemic. Biden said “the irony” is he’s probably been able to reach more voters through virtual campaigning.“So far, it remains to be seen, I don’t want to jinx myself, I know the polling data is very good. But I think it’s really early. It’s much too early to make any judgment,” Biden said.Biden in the basement: Can campaigning from home work as Trump starts to travel?Trump and Republicans have struggled to find an attack against Biden that’s stuck.During a conference call with reporters, Trump communication director Tim Murtaugh threw the gauntlet at Biden.He slammed Biden for not denouncing the tear-downs of monuments by protesters, called him a “disaster” on the economy, talked extensively about Rep. Alexandria Ocasio-Cortez, D-N.Y., questioned Biden’s ties to China and argued the Obama-Biden administration’s handling of the H1N1 pandemic left Trump with a shortage of N95 masks. He accused Biden of using COVID-19 as a “political weapon in a cynical attempt” to undermine public confidence.“Joe Biden is hoping to ride out the rest of these four months without taking any of these questions,” Murtaugh said. “He’s not undergoing thorough vetting before the American people, and he’s not facing scrutiny because his handlers know he is not up to it.”Comparing the 2020 and 2016 elections, Robby Mook, Clinton's 2016 campaign manager, said last week, “I almost look at it as: Is there very much that’s the same?” He appeared on the podcast of David Plouffe, Barack Obama’s former campaign manager. “First and foremost, I’d say COVID has changed everything.”Mook, president of the House Majority PAC, said Trump is taken "more seriously" and "being held to account in a way that he wasn’t in ’16.” Whereas Trump’s "petty" remarks were treated as a “novelty” in 2016, they’re now seen “in a context of a true lack of leadership,” he said. Political experience tends to be a liability in campaigns, Mook said, but it’s viewed as a strength for Biden during the pandemic. “I think Hillary kind of got the opposite end of that." He predicted the race would tighten up as voters, as they historically do, "go home to their parties," but not if Trump can't "get his act together."“Biden wants this to be a referendum on Trump, and he’s winning that right now. Trump needs to reengineer that to be a choice – and he can’t even offer what that choice is," Mook said. "So how in the world are they supposed to get this on firmer ground for their strategy?”None of the Trump taglines on Biden has gained traction like “Crooked Hillary” and chants of “Lock her up” four years ago.Democrats, despite their cautious optimism, are bullish about the issues being in their favor: a pandemic they contend exposed failed presidential leadership and Trump's “law and order” response to protests over systemic racism and police brutality as polling shows more Americans are favorable to the Black Lives Matter movement. "We understand what the temperature and the pulse of the country looks like right now,” said Shelia Huggins, an attorney from Durham, North Carolina, and DNC committee member.More:Joe Biden campaign seizes on opportunity to contrast Trump's 'law and order' messageShe said her Democratic friends aren’t talking about a 2016 repeat as much as they once were."We’re too busy listening to a president who is talking nonsense pretty much every day,” she said. “You're easily reminded that 2016 is not what needs to be on the forefront of what we're thinking about. We need to be thinking about 2020."In Arizona, Heredia said he believes Democrats have momentum to carry the state for Biden, win the U.S. Senate race between Democrat Mark Kelly and Sen. Martha McSally and flip both chambers of the state Legislature, where Republicans have slim majorities. The last Democrat to carry Arizona for president was Bill Clinton in 1996. “There's a perfect storm building up in Arizona, I would call it a perfect ‘haboob’ in our state,” he said, referring to the dust storms that pop up in the SouthwestMore:Trump calls proposed Black Lives Matter mural outside Trump Tower 'a symbol of hate'Ken Evans, a DNC committee member from Florida, who runs a camp for children in Fort Lauderdale, said he knows many "nonpartisan people" in Broward County who voted for Trump because they couldn’t back Clinton, but they plan to vote for Biden in November. He said the president’s handling of the coronavirus was the last straw.“That’s making the difference. That’s what’s going to bring out the vote,” Evans said, defending voter enthusiasm for Biden. “They’re excited to bring normalcy back to the White House” after all the "tiresome" Trump drama, he said. “People are tired.”When it comes to Biden being ahead in polls, though, Evans returned to four years ago.“So was Hillary, right?” he said.Reach Joey Garrison on Twitter @joeygarrison.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RE:ブルーススプリングスティーンの大ヒット曲 『Born in the USA』の歌詞の中で 『ベトナムに黄色い猿を殺しに行く』ってフレーズが あるんですけど、スプリングスティーンさんて 人種差別主...</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Source: カテゴリ一覧 - Yahoo!知恵袋Forum: 洋楽</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://detail.chiebukuro.yahoo.co.jp/qa/question_detail/q14227811489</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>コロナ給付金寄付プロジェクト「あなたの思いをあしたの支援に」検索IDでもっと便利に新規取得ログイン送料込み1,000円、目玉商品セール中条件指定質問・相談回答受付終了まであと4日　回答を投稿すると知恵コイン15枚が追加されますシェアツイートはてブ知恵コレID非公開さん2020/7/312:35:55ブルーススプリングスティーンの大ヒット曲
+『Born in the USA』の歌詞の中で
+『ベトナムに黄色い猿を殺しに行く』ってフレーズが
+あるんですけど、スプリングスティーンさんて人種差別主義者なんですか？違反報告回答投稿シェアツイートはてブ知恵コレ1〜5件/5件中猿メガネさん編集あり2020/7/517:01:15仮に黄色い猿と歌ってたとしても
+前後の文脈をしっかり聴けば
+人種差別主義者なんかでは
+ないことが理解できるはず。
+ある単語やフレーズだけを抜き出して
+過剰に反応する
+リテラシー能力のない人が
+最近は多いみたいやけど。違反報告kus********さん2020/7/319:45:27妄想が過ぎます違反報告不適切な内容が含まれている可能性があるため、非表示になっています。投稿内容に関する注意つぃんどっぐさん2020/7/314:41:04Got in a little hometown jam so they put rifle in my hand.
+Sent me off to a foriegan land to go and kill the yellow man.
+Born in the U.S.A.
+I was born in the U.S.A.
+.....
+どこにもyellow monkyとは書いてないが?違反報告質問者ID非公開さん2020/7/315:16:53Got in a little hometown jam
+So they put a rifle in my hand
+Sent me off to a foreign land
+To go and kill the yellow mon
+https://blog.goo.ne.jp/kantenbou/e/3bb6da51509f89f43922a62d2371fc7f
+書いてるじゃないか？違反報告その他の返信（3件）を表示ave********さん2020/7/312:48:03「黄色い猿」なんて歌っていません、「黄色い人間」の間違いです。
+人種をイエローというのは、そんなに差別的じゃないでしょう。違反報告一覧を見るみんなで作る知恵袋　悩みや疑問、なんでも気軽にきいちゃおう！Q&amp;Aをキーワードで検索：ランキングをもっと見る一覧を見るエンターテインメントと趣味∟音楽JASRAC許諾番号：9008249113Y38200Copyright (C) 2020 Yahoo Japan Corporation. All Rights Reserved.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>WTTF: Team USA Cards</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Source: Sports Card Trading and Sports Card ForumForum: Most Recent SCF Posts</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://www.sportscardforum.com/threads/2521884-WTTF-Team-USA-Cards</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Re: Anytown, USA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Source: The Motley Fool Discussion BoardsForum: Political Asylum</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://boards.fool.com/Message.aspx?mid=34552208&amp;sort=whole</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Folders | Best Of | Favorites &amp; Replies | Settings | Start a New Board | My Fool | Help |© 1995 - 2020 The Motley Fool. All rights reserved.
+Market data powered by FactSet and Web Financial Group.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>www.validdocumentsonline.com BUY REAL PASSPORTS / USA PASSPO</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Source: AboutAlcoholismForum: 12-Step Recovery</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>http://aboutalcoholism.proboards.com/post/5187/thread</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Welcome Guest. Please Login or Register.Welcome Guest. Please Login or Register.</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">

</xml_diff>